<commit_message>
pesky pikes need some coaxing to show up consistently trying image zooming; not liking it; need better quality images of monsters can now add match string on the fly saving enemies.xml to desktop after app closes verified gp/xp for enemies up to mt. hobs
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -138,18 +138,12 @@
     <t>Aligator</t>
   </si>
   <si>
-    <t>Mad Toad</t>
-  </si>
-  <si>
     <t>Mist Dragon</t>
   </si>
   <si>
     <t>Octomamm</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>GP</t>
   </si>
   <si>
@@ -165,120 +159,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Watery Pass Floor B1F/B2F -017</t>
-  </si>
-  <si>
-    <t>-------------------------</t>
-  </si>
-  <si>
-    <t>01: 012(00C): EvilShel x3  WaterBug x1</t>
-  </si>
-  <si>
-    <t>02: 013(00D): Pike     x3</t>
-  </si>
-  <si>
-    <t>03: 014(00E): CaveToad x3</t>
-  </si>
-  <si>
-    <t>04: 015(00F): Pike     x2, EvilShel x2</t>
-  </si>
-  <si>
-    <t>05: 012(00C): EvilShel x3, WaterBug x1</t>
-  </si>
-  <si>
-    <t>06: 013(00D): Pike     x3</t>
-  </si>
-  <si>
-    <t>07: 016(010): Zombie   x4</t>
-  </si>
-  <si>
-    <t>08: 016(010): Zombie   x4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watery Pass  B3F -018 </t>
-  </si>
-  <si>
-    <t>----------------</t>
-  </si>
-  <si>
-    <t>01: 013(00D): Pike     x3</t>
-  </si>
-  <si>
-    <t>02: 014(00E): CaveToad x3</t>
-  </si>
-  <si>
-    <t>03: 015(00F): Pike     x2, EvilShel x2</t>
-  </si>
-  <si>
-    <t>04: 016(010): Zombie   x4</t>
-  </si>
-  <si>
-    <t>05: 017(011): Pike     x2, EvilShel x2, WaterBug x2</t>
-  </si>
-  <si>
-    <t>06: 018(012): Jelly    x4</t>
-  </si>
-  <si>
-    <t>07: 019(013): TinyMage x2, WaterHag x4</t>
-  </si>
-  <si>
-    <t>08: 019(013): TinyMage x2, WaterHag x4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watery Pass North -019 </t>
-  </si>
-  <si>
-    <t>-----------------</t>
-  </si>
-  <si>
-    <t>01: 016(010): Zombie   x4</t>
-  </si>
-  <si>
-    <t>02: 017(011): Pike     x2, EvilShel x2, WaterBug x2</t>
-  </si>
-  <si>
-    <t>03: 018(012): Jelly    x4</t>
-  </si>
-  <si>
-    <t>04: 020(014): CaveToad x4</t>
-  </si>
-  <si>
-    <t>05: 021(015): CaveToad x2, Mad Toad x2</t>
-  </si>
-  <si>
-    <t>06: 022(016): Aligator x1, Pike x2</t>
-  </si>
-  <si>
-    <t>Watery Pass Waterfalls -020</t>
-  </si>
-  <si>
-    <t>----------------------</t>
-  </si>
-  <si>
-    <t>01: 018(012): Jelly    x4</t>
-  </si>
-  <si>
-    <t>02: 022(016): Aligator x1, Pike     x2</t>
-  </si>
-  <si>
-    <t>03: 019(013): TinyMage x2, WaterHag x4</t>
-  </si>
-  <si>
-    <t>04: 024(018): Zombie   x6</t>
-  </si>
-  <si>
-    <t>05: 023(017): Aligator x2</t>
-  </si>
-  <si>
-    <t>06: 025(019): Aligator x1, WaterBug x2</t>
-  </si>
-  <si>
-    <t>07: 026(01A): Mad Toad x4</t>
-  </si>
-  <si>
-    <t>08: 027(01B): TinyMage x4</t>
-  </si>
-  <si>
     <t>MadToad</t>
   </si>
   <si>
@@ -286,6 +166,123 @@
   </si>
   <si>
     <t>Soldier</t>
+  </si>
+  <si>
+    <t>06: 036(024): Turtle   x2</t>
+  </si>
+  <si>
+    <t>---------------</t>
+  </si>
+  <si>
+    <t>Imp Cap.</t>
+  </si>
+  <si>
+    <t>Basilisk</t>
+  </si>
+  <si>
+    <t>Turtle</t>
+  </si>
+  <si>
+    <t>Weeper</t>
+  </si>
+  <si>
+    <t>Cream</t>
+  </si>
+  <si>
+    <t>Antlion</t>
+  </si>
+  <si>
+    <t>Mt. Hobs West -023</t>
+  </si>
+  <si>
+    <t>-------------</t>
+  </si>
+  <si>
+    <t>01: 040(028): Skelton  x4</t>
+  </si>
+  <si>
+    <t>02: 041(029): Spirit   x2</t>
+  </si>
+  <si>
+    <t>03: 042(02A): Gargoyle x1, Cocktric x2</t>
+  </si>
+  <si>
+    <t>04: 043(02B): Bomb     x3</t>
+  </si>
+  <si>
+    <t>05: 044(02C): Cocktric x3</t>
+  </si>
+  <si>
+    <t>06: 045(02D): Gargoyle x2</t>
+  </si>
+  <si>
+    <t>07: 046(02E): GrayBomb x2, Bomb     x2</t>
+  </si>
+  <si>
+    <t>08: 046(02E): GrayBomb x2, Bomb     x2</t>
+  </si>
+  <si>
+    <t>Mt. Hobs Summit -024</t>
+  </si>
+  <si>
+    <t>01: 042(02A): Gargoyle x1, Cocktric x2</t>
+  </si>
+  <si>
+    <t>03: 046(02E): GrayBomb x2, Bomb     x2</t>
+  </si>
+  <si>
+    <t>04: 040(028): Skelton  x4</t>
+  </si>
+  <si>
+    <t>06: 047(02F): Spirit   x2, Skelton  x2</t>
+  </si>
+  <si>
+    <t>07: 045(02D): Gargoyle x2</t>
+  </si>
+  <si>
+    <t>08: 051(033): Spirit   x3, Skelton  x2, Red Bone x1</t>
+  </si>
+  <si>
+    <t>Mt. Hobs East -025</t>
+  </si>
+  <si>
+    <t>01: 047(02F): Spirit   x2, Skelton x2</t>
+  </si>
+  <si>
+    <t>02: 045(02D): Gargoyle x2</t>
+  </si>
+  <si>
+    <t>03: 046(02E): GrayBomb x2, Bomb x2</t>
+  </si>
+  <si>
+    <t>04: 042(02A): Gargoyle x1, Cocktric x1</t>
+  </si>
+  <si>
+    <t>05: 049(031): Red Bone x1, Skelton x3</t>
+  </si>
+  <si>
+    <t>08: 050(032): GrayBomb x2, Bomb x4</t>
+  </si>
+  <si>
+    <t>Skelton</t>
+  </si>
+  <si>
+    <t>Spirit</t>
+  </si>
+  <si>
+    <t>Gargoyle</t>
+  </si>
+  <si>
+    <t>Cocktric</t>
+  </si>
+  <si>
+    <t>Bomb</t>
+  </si>
+  <si>
+    <t>GrayBomb</t>
+  </si>
+  <si>
+    <t>Red Bone</t>
   </si>
 </sst>
 </file>
@@ -341,8 +338,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="H1:J23" totalsRowShown="0">
-  <autoFilter ref="H1:J23" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C37" totalsRowShown="0">
+  <autoFilter ref="A1:C37" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92B7C1DE-0885-429F-9F5C-CD5B673ABB7F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4EFBCB72-C5CC-4F4D-973E-B96095039970}" name="GP"/>
@@ -649,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:D19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,382 +661,459 @@
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2">
+      <c r="B4">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5">
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
         <v>20</v>
       </c>
-      <c r="J5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7">
-        <v>20</v>
-      </c>
-      <c r="J7">
+      <c r="C7">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>700</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>120</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>110</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>230</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>140</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>500</v>
+      </c>
+      <c r="C18">
+        <v>1200</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>260</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>140</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>130</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>80</v>
+      </c>
+      <c r="C22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>160</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24">
+        <v>95</v>
+      </c>
+      <c r="C24">
+        <v>240</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>190</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>120</v>
+      </c>
+      <c r="E26" t="s">
         <v>74</v>
       </c>
-      <c r="H8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8">
-        <v>200</v>
-      </c>
-      <c r="J8">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>80</v>
+      </c>
+      <c r="C27">
+        <v>240</v>
+      </c>
+      <c r="E27" t="s">
         <v>75</v>
       </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9">
-        <v>20</v>
-      </c>
-      <c r="J9">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>160</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>150</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>800</v>
+      </c>
+      <c r="C30">
+        <v>1500</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10">
-        <v>25</v>
-      </c>
-      <c r="J10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11">
-        <v>25</v>
-      </c>
-      <c r="J11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="E32" t="s">
         <v>78</v>
       </c>
-      <c r="H12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12">
-        <v>35</v>
-      </c>
-      <c r="J12">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13">
-        <v>30</v>
-      </c>
-      <c r="J13">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14">
-        <v>80</v>
-      </c>
-      <c r="J14">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>81</v>
       </c>
-      <c r="H15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>82</v>
       </c>
-      <c r="H16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>83</v>
       </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>85</v>
-      </c>
-      <c r="I22">
-        <v>80</v>
-      </c>
-      <c r="J22">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
-        <v>86</v>
-      </c>
-      <c r="I23">
-        <v>55</v>
-      </c>
-      <c r="J23">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>59</v>
-      </c>
-      <c r="I28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>60</v>
-      </c>
-      <c r="I29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" t="s">
-        <v>64</v>
-      </c>
-      <c r="I33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trimmed some old code that is no longer used updated some enemy match strings added special case where M is recognized as h refactored line processing to work more directly with strings added and verified most of Mt. Ordeals enemy data; was very wrong in both sources Enemy Clear button now also clears enemy UI groups
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="123">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -168,12 +168,6 @@
     <t>Soldier</t>
   </si>
   <si>
-    <t>06: 036(024): Turtle   x2</t>
-  </si>
-  <si>
-    <t>---------------</t>
-  </si>
-  <si>
     <t>Imp Cap.</t>
   </si>
   <si>
@@ -192,78 +186,6 @@
     <t>Antlion</t>
   </si>
   <si>
-    <t>Mt. Hobs West -023</t>
-  </si>
-  <si>
-    <t>-------------</t>
-  </si>
-  <si>
-    <t>01: 040(028): Skelton  x4</t>
-  </si>
-  <si>
-    <t>02: 041(029): Spirit   x2</t>
-  </si>
-  <si>
-    <t>03: 042(02A): Gargoyle x1, Cocktric x2</t>
-  </si>
-  <si>
-    <t>04: 043(02B): Bomb     x3</t>
-  </si>
-  <si>
-    <t>05: 044(02C): Cocktric x3</t>
-  </si>
-  <si>
-    <t>06: 045(02D): Gargoyle x2</t>
-  </si>
-  <si>
-    <t>07: 046(02E): GrayBomb x2, Bomb     x2</t>
-  </si>
-  <si>
-    <t>08: 046(02E): GrayBomb x2, Bomb     x2</t>
-  </si>
-  <si>
-    <t>Mt. Hobs Summit -024</t>
-  </si>
-  <si>
-    <t>01: 042(02A): Gargoyle x1, Cocktric x2</t>
-  </si>
-  <si>
-    <t>03: 046(02E): GrayBomb x2, Bomb     x2</t>
-  </si>
-  <si>
-    <t>04: 040(028): Skelton  x4</t>
-  </si>
-  <si>
-    <t>06: 047(02F): Spirit   x2, Skelton  x2</t>
-  </si>
-  <si>
-    <t>07: 045(02D): Gargoyle x2</t>
-  </si>
-  <si>
-    <t>08: 051(033): Spirit   x3, Skelton  x2, Red Bone x1</t>
-  </si>
-  <si>
-    <t>Mt. Hobs East -025</t>
-  </si>
-  <si>
-    <t>01: 047(02F): Spirit   x2, Skelton x2</t>
-  </si>
-  <si>
-    <t>02: 045(02D): Gargoyle x2</t>
-  </si>
-  <si>
-    <t>03: 046(02E): GrayBomb x2, Bomb x2</t>
-  </si>
-  <si>
-    <t>04: 042(02A): Gargoyle x1, Cocktric x1</t>
-  </si>
-  <si>
-    <t>05: 049(031): Red Bone x1, Skelton x3</t>
-  </si>
-  <si>
-    <t>08: 050(032): GrayBomb x2, Bomb x4</t>
-  </si>
-  <si>
     <t>Skelton</t>
   </si>
   <si>
@@ -283,6 +205,195 @@
   </si>
   <si>
     <t>Red Bone</t>
+  </si>
+  <si>
+    <t>Needler</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Dragoon appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mysidia Landscape -004 </t>
+  </si>
+  <si>
+    <t>-----------------</t>
+  </si>
+  <si>
+    <t>01: 056(038): Raven    x1</t>
+  </si>
+  <si>
+    <t>02: 029(01D): SwordRat x2, Imp      x2, TinyMage x2</t>
+  </si>
+  <si>
+    <t>03: 052(034): Imp Cap. x3, Needler  x1</t>
+  </si>
+  <si>
+    <t>04: 054(036): Imp Cap. x4, Imp      x2</t>
+  </si>
+  <si>
+    <t>05: 056(038): Raven    x1</t>
+  </si>
+  <si>
+    <t>06: 058(03A): Needler  x2, SwordRat x2</t>
+  </si>
+  <si>
+    <t>07: 088(058): Raven    x1, Cocktric x3</t>
+  </si>
+  <si>
+    <t>08: 088(058): Raven    x1, Cocktric x3</t>
+  </si>
+  <si>
+    <t>Mt. Ordeals -026</t>
+  </si>
+  <si>
+    <t>-----------</t>
+  </si>
+  <si>
+    <t>01: 047(02F): Spirit   x2, Skelton  x2</t>
+  </si>
+  <si>
+    <t>02: 049(031): Red Bone x1, Skelton  x3</t>
+  </si>
+  <si>
+    <t>03: 051(033): Spirit   x3, Skelton  x2, Red Bone x1</t>
+  </si>
+  <si>
+    <t>04: 060(03C): Spirit   x3, Soul     x1</t>
+  </si>
+  <si>
+    <t>05: 061(03D): Soul     x2, Red Bone x2</t>
+  </si>
+  <si>
+    <t>06: 062(03E): Skelton  x3, Red Bone x2</t>
+  </si>
+  <si>
+    <t>07: 063(03F): Lilith   x1, Red Bone x2</t>
+  </si>
+  <si>
+    <t>08: 063(03F): Lilith   x1, Red Bone x2</t>
+  </si>
+  <si>
+    <t>Mt. Ordeals 3rd Station -027</t>
+  </si>
+  <si>
+    <t>-----------------------</t>
+  </si>
+  <si>
+    <t>01: 064(040): Ghoul    x1, Red Bone x2, Skelton  x2</t>
+  </si>
+  <si>
+    <t>02: 065(041): Spirit   x2, Soul     x2, Red Bone x2</t>
+  </si>
+  <si>
+    <t>03: 066(042): Zombie   x2, Ghoul    x2</t>
+  </si>
+  <si>
+    <t>04: 067(043): Ghoul    x2, Soul     x2</t>
+  </si>
+  <si>
+    <t>05: 068(044): Revenant x1, Ghoul    x3</t>
+  </si>
+  <si>
+    <t>06: 069(045): Zombie   x3, Ghoul    x2, Revenant x2</t>
+  </si>
+  <si>
+    <t>Mt. Ordeals 7th Station/Summit -028</t>
+  </si>
+  <si>
+    <t>------------------------------</t>
+  </si>
+  <si>
+    <t>01: 067(043): Ghoul    x2, Soul     x2</t>
+  </si>
+  <si>
+    <t>02: 068(044): Revenant x1, Ghoul    x3</t>
+  </si>
+  <si>
+    <t>03: 069(045): Zombie   x3, Ghoul    x2, Revenant x2</t>
+  </si>
+  <si>
+    <t>04: 071(047): Soul     x2, Ghoul    x2, Revenant x2</t>
+  </si>
+  <si>
+    <t>05: 063(03F): Lilith   x1, Red Bone x2</t>
+  </si>
+  <si>
+    <t>06: 070(046): Lilith   x1</t>
+  </si>
+  <si>
+    <t>07: 072(048): Soul     x3, Ghoul    x1, Revenant x1</t>
+  </si>
+  <si>
+    <t>08: 073(049): Lilith   x2</t>
+  </si>
+  <si>
+    <t>Raven</t>
+  </si>
+  <si>
+    <t>2 soul</t>
+  </si>
+  <si>
+    <t>2 red bone</t>
+  </si>
+  <si>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Soul</t>
+  </si>
+  <si>
+    <t>3 spirit</t>
+  </si>
+  <si>
+    <t>2 skelton</t>
+  </si>
+  <si>
+    <t>red bone</t>
+  </si>
+  <si>
+    <t>soul</t>
+  </si>
+  <si>
+    <t>revenant</t>
+  </si>
+  <si>
+    <t>3 ghoul</t>
+  </si>
+  <si>
+    <t>3 soul</t>
+  </si>
+  <si>
+    <t>ghoul</t>
+  </si>
+  <si>
+    <t>lilith</t>
+  </si>
+  <si>
+    <t>Lilith</t>
+  </si>
+  <si>
+    <t>3 zombie</t>
+  </si>
+  <si>
+    <t>2 ghoul</t>
+  </si>
+  <si>
+    <t>2 revenant</t>
+  </si>
+  <si>
+    <t>Ghoul</t>
+  </si>
+  <si>
+    <t>Revenant</t>
   </si>
 </sst>
 </file>
@@ -318,8 +429,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,12 +450,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C37" totalsRowShown="0">
-  <autoFilter ref="A1:C37" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0">
+  <autoFilter ref="A1:C38" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92B7C1DE-0885-429F-9F5C-CD5B673ABB7F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4EFBCB72-C5CC-4F4D-973E-B96095039970}" name="GP"/>
     <tableColumn id="3" xr3:uid="{76E6ED1B-435E-45FF-A3AA-315C85BADFCD}" name="Experience"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G38" totalsRowShown="0">
+  <autoFilter ref="E1:G38" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{7A239594-29E1-43D2-A7C7-BAD18B95F548}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{88D0DB9C-FE4B-4B88-80D2-A005BCE333DB}" name="GP"/>
+    <tableColumn id="3" xr3:uid="{2B5D719C-C423-461E-AF1F-B7F661772F51}" name="Experience"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -646,22 +770,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -672,10 +797,19 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -686,10 +820,19 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F2">
+        <v>55</v>
+      </c>
+      <c r="G2">
+        <v>370</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -700,10 +843,19 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>410</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -714,10 +866,19 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F4">
+        <v>155</v>
+      </c>
+      <c r="G4">
+        <v>610</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -728,10 +889,16 @@
         <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -742,10 +909,23 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="F6">
+        <v>165</v>
+      </c>
+      <c r="G6">
+        <v>510</v>
+      </c>
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -756,10 +936,23 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F7">
+        <v>170</v>
+      </c>
+      <c r="G7">
+        <v>320</v>
+      </c>
+      <c r="K7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -770,10 +963,19 @@
         <v>700</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F8">
+        <v>125</v>
+      </c>
+      <c r="G8">
+        <v>290</v>
+      </c>
+      <c r="K8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -784,10 +986,19 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="F9">
+        <v>365</v>
+      </c>
+      <c r="G9">
+        <v>2750</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -798,10 +1009,19 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="F10">
+        <v>180</v>
+      </c>
+      <c r="G10">
+        <v>580</v>
+      </c>
+      <c r="K10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -811,8 +1031,17 @@
       <c r="C11">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11">
+        <v>190</v>
+      </c>
+      <c r="G11">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -822,11 +1051,14 @@
       <c r="C12">
         <v>120</v>
       </c>
-      <c r="E12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -836,11 +1068,14 @@
       <c r="C13">
         <v>110</v>
       </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -850,11 +1085,14 @@
       <c r="C14">
         <v>230</v>
       </c>
-      <c r="E14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -864,11 +1102,14 @@
       <c r="C15">
         <v>90</v>
       </c>
-      <c r="E15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -878,11 +1119,14 @@
       <c r="C16">
         <v>120</v>
       </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -892,11 +1136,14 @@
       <c r="C17">
         <v>140</v>
       </c>
-      <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -906,11 +1153,14 @@
       <c r="C18">
         <v>1200</v>
       </c>
-      <c r="E18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -920,11 +1170,14 @@
       <c r="C19">
         <v>260</v>
       </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -934,11 +1187,14 @@
       <c r="C20">
         <v>140</v>
       </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -948,11 +1204,14 @@
       <c r="C21">
         <v>130</v>
       </c>
-      <c r="E21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -963,7 +1222,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -973,11 +1232,11 @@
       <c r="C23">
         <v>160</v>
       </c>
-      <c r="E23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -987,13 +1246,13 @@
       <c r="C24">
         <v>240</v>
       </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -1001,13 +1260,13 @@
       <c r="C25">
         <v>190</v>
       </c>
-      <c r="E25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>30</v>
@@ -1015,13 +1274,25 @@
       <c r="C26">
         <v>120</v>
       </c>
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>87</v>
+      </c>
+      <c r="S26" t="s">
+        <v>105</v>
+      </c>
+      <c r="T26" t="s">
+        <v>106</v>
+      </c>
+      <c r="W26" t="s">
+        <v>105</v>
+      </c>
+      <c r="X26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B27">
         <v>80</v>
@@ -1029,13 +1300,27 @@
       <c r="C27">
         <v>240</v>
       </c>
-      <c r="E27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>88</v>
+      </c>
+      <c r="R27" t="s">
+        <v>103</v>
+      </c>
+      <c r="V27" t="s">
+        <v>108</v>
+      </c>
+      <c r="W27">
+        <f>W30/3</f>
+        <v>125</v>
+      </c>
+      <c r="X27">
+        <f>X30/3</f>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28">
         <v>40</v>
@@ -1043,13 +1328,27 @@
       <c r="C28">
         <v>160</v>
       </c>
-      <c r="E28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>89</v>
+      </c>
+      <c r="R28" t="s">
+        <v>104</v>
+      </c>
+      <c r="V28" t="s">
+        <v>111</v>
+      </c>
+      <c r="W28">
+        <f>F6</f>
+        <v>165</v>
+      </c>
+      <c r="X28">
+        <f>G6</f>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29">
         <v>35</v>
@@ -1057,13 +1356,19 @@
       <c r="C29">
         <v>150</v>
       </c>
-      <c r="E29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>90</v>
+      </c>
+      <c r="W29">
+        <v>540</v>
+      </c>
+      <c r="X29">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>800</v>
@@ -1071,55 +1376,157 @@
       <c r="C30">
         <v>1500</v>
       </c>
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>91</v>
+      </c>
+      <c r="W30">
+        <f>W29-W28</f>
+        <v>375</v>
+      </c>
+      <c r="X30">
+        <f>X29-X28</f>
+        <v>870</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="K31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="K32" t="s">
+        <v>83</v>
+      </c>
+      <c r="R32" t="s">
+        <v>108</v>
+      </c>
+      <c r="V32" t="s">
+        <v>112</v>
+      </c>
+      <c r="W32">
+        <f>F11</f>
+        <v>190</v>
+      </c>
+      <c r="X32">
+        <f>G11</f>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="R33" t="s">
+        <v>109</v>
+      </c>
+      <c r="V33" t="s">
+        <v>113</v>
+      </c>
+      <c r="W33">
+        <f>3*F10</f>
+        <v>540</v>
+      </c>
+      <c r="X33">
+        <f>3*G10</f>
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="R34" t="s">
+        <v>110</v>
+      </c>
+      <c r="V34">
+        <v>4</v>
+      </c>
+      <c r="W34">
+        <f>W33+W32</f>
+        <v>730</v>
+      </c>
+      <c r="X34">
+        <f>X33+X32</f>
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="V35">
+        <v>1</v>
+      </c>
+      <c r="X35">
+        <f>X34/4</f>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>59</v>
+      </c>
+      <c r="R37" t="s">
+        <v>114</v>
+      </c>
+      <c r="V37" t="s">
+        <v>116</v>
+      </c>
+      <c r="W37">
+        <v>365</v>
+      </c>
+      <c r="X37">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R38" t="s">
+        <v>112</v>
+      </c>
+      <c r="V38">
+        <v>4</v>
+      </c>
+      <c r="X38">
+        <f>2750/4</f>
+        <v>687.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R44" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
filter out fast forwards from string matching added data for milon, milon z. rudimentary checks to differentiate milon, milon z. condensed match string distinction
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t>Revenant</t>
+  </si>
+  <si>
+    <t>Milon</t>
+  </si>
+  <si>
+    <t>Ghast</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Milon Z.</t>
   </si>
 </sst>
 </file>
@@ -773,7 +785,7 @@
   <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,6 +1063,18 @@
       <c r="C12">
         <v>120</v>
       </c>
+      <c r="E12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12">
+        <v>3000</v>
+      </c>
+      <c r="G12">
+        <v>3000</v>
+      </c>
+      <c r="H12" t="s">
+        <v>125</v>
+      </c>
       <c r="K12" t="s">
         <v>74</v>
       </c>
@@ -1068,6 +1092,18 @@
       <c r="C13">
         <v>110</v>
       </c>
+      <c r="E13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13">
+        <v>75</v>
+      </c>
+      <c r="G13">
+        <v>800</v>
+      </c>
+      <c r="H13" t="s">
+        <v>125</v>
+      </c>
       <c r="K13" t="s">
         <v>75</v>
       </c>
@@ -1084,6 +1120,15 @@
       </c>
       <c r="C14">
         <v>230</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14">
+        <v>3000</v>
+      </c>
+      <c r="G14">
+        <v>4000</v>
       </c>
       <c r="K14" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
converted string filtering to regex, since i care only about letters (and possibly numbers for items, if i can get them to recognize) filled in enemy data for mt. hobs completed enemy data through kainazzo
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -219,177 +219,15 @@
     <t>Dragoon appears</t>
   </si>
   <si>
-    <t xml:space="preserve">Mysidia Landscape -004 </t>
-  </si>
-  <si>
-    <t>-----------------</t>
-  </si>
-  <si>
-    <t>01: 056(038): Raven    x1</t>
-  </si>
-  <si>
-    <t>02: 029(01D): SwordRat x2, Imp      x2, TinyMage x2</t>
-  </si>
-  <si>
-    <t>03: 052(034): Imp Cap. x3, Needler  x1</t>
-  </si>
-  <si>
-    <t>04: 054(036): Imp Cap. x4, Imp      x2</t>
-  </si>
-  <si>
-    <t>05: 056(038): Raven    x1</t>
-  </si>
-  <si>
-    <t>06: 058(03A): Needler  x2, SwordRat x2</t>
-  </si>
-  <si>
-    <t>07: 088(058): Raven    x1, Cocktric x3</t>
-  </si>
-  <si>
-    <t>08: 088(058): Raven    x1, Cocktric x3</t>
-  </si>
-  <si>
-    <t>Mt. Ordeals -026</t>
-  </si>
-  <si>
-    <t>-----------</t>
-  </si>
-  <si>
-    <t>01: 047(02F): Spirit   x2, Skelton  x2</t>
-  </si>
-  <si>
-    <t>02: 049(031): Red Bone x1, Skelton  x3</t>
-  </si>
-  <si>
-    <t>03: 051(033): Spirit   x3, Skelton  x2, Red Bone x1</t>
-  </si>
-  <si>
-    <t>04: 060(03C): Spirit   x3, Soul     x1</t>
-  </si>
-  <si>
-    <t>05: 061(03D): Soul     x2, Red Bone x2</t>
-  </si>
-  <si>
-    <t>06: 062(03E): Skelton  x3, Red Bone x2</t>
-  </si>
-  <si>
-    <t>07: 063(03F): Lilith   x1, Red Bone x2</t>
-  </si>
-  <si>
-    <t>08: 063(03F): Lilith   x1, Red Bone x2</t>
-  </si>
-  <si>
-    <t>Mt. Ordeals 3rd Station -027</t>
-  </si>
-  <si>
-    <t>-----------------------</t>
-  </si>
-  <si>
-    <t>01: 064(040): Ghoul    x1, Red Bone x2, Skelton  x2</t>
-  </si>
-  <si>
-    <t>02: 065(041): Spirit   x2, Soul     x2, Red Bone x2</t>
-  </si>
-  <si>
-    <t>03: 066(042): Zombie   x2, Ghoul    x2</t>
-  </si>
-  <si>
-    <t>04: 067(043): Ghoul    x2, Soul     x2</t>
-  </si>
-  <si>
-    <t>05: 068(044): Revenant x1, Ghoul    x3</t>
-  </si>
-  <si>
-    <t>06: 069(045): Zombie   x3, Ghoul    x2, Revenant x2</t>
-  </si>
-  <si>
-    <t>Mt. Ordeals 7th Station/Summit -028</t>
-  </si>
-  <si>
-    <t>------------------------------</t>
-  </si>
-  <si>
-    <t>01: 067(043): Ghoul    x2, Soul     x2</t>
-  </si>
-  <si>
-    <t>02: 068(044): Revenant x1, Ghoul    x3</t>
-  </si>
-  <si>
-    <t>03: 069(045): Zombie   x3, Ghoul    x2, Revenant x2</t>
-  </si>
-  <si>
-    <t>04: 071(047): Soul     x2, Ghoul    x2, Revenant x2</t>
-  </si>
-  <si>
-    <t>05: 063(03F): Lilith   x1, Red Bone x2</t>
-  </si>
-  <si>
-    <t>06: 070(046): Lilith   x1</t>
-  </si>
-  <si>
-    <t>07: 072(048): Soul     x3, Ghoul    x1, Revenant x1</t>
-  </si>
-  <si>
-    <t>08: 073(049): Lilith   x2</t>
-  </si>
-  <si>
     <t>Raven</t>
   </si>
   <si>
-    <t>2 soul</t>
-  </si>
-  <si>
-    <t>2 red bone</t>
-  </si>
-  <si>
-    <t>gp</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
     <t>Soul</t>
   </si>
   <si>
-    <t>3 spirit</t>
-  </si>
-  <si>
-    <t>2 skelton</t>
-  </si>
-  <si>
-    <t>red bone</t>
-  </si>
-  <si>
-    <t>soul</t>
-  </si>
-  <si>
-    <t>revenant</t>
-  </si>
-  <si>
-    <t>3 ghoul</t>
-  </si>
-  <si>
-    <t>3 soul</t>
-  </si>
-  <si>
-    <t>ghoul</t>
-  </si>
-  <si>
-    <t>lilith</t>
-  </si>
-  <si>
     <t>Lilith</t>
   </si>
   <si>
-    <t>3 zombie</t>
-  </si>
-  <si>
-    <t>2 ghoul</t>
-  </si>
-  <si>
-    <t>2 revenant</t>
-  </si>
-  <si>
     <t>Ghoul</t>
   </si>
   <si>
@@ -406,6 +244,33 @@
   </si>
   <si>
     <t>Milon Z.</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>Piranha</t>
+  </si>
+  <si>
+    <t>FangShel</t>
+  </si>
+  <si>
+    <t>Crocdile</t>
+  </si>
+  <si>
+    <t>ElecFish</t>
+  </si>
+  <si>
+    <t>AquaWorm</t>
+  </si>
+  <si>
+    <t>Hydra</t>
+  </si>
+  <si>
+    <t>Baigan</t>
+  </si>
+  <si>
+    <t>Kainazzo</t>
   </si>
 </sst>
 </file>
@@ -448,7 +313,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -462,8 +338,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0">
-  <autoFilter ref="A1:C38" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0">
+  <autoFilter ref="A1:C36" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92B7C1DE-0885-429F-9F5C-CD5B673ABB7F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4EFBCB72-C5CC-4F4D-973E-B96095039970}" name="GP"/>
@@ -474,8 +350,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G38" totalsRowShown="0">
-  <autoFilter ref="E1:G38" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G37" totalsRowShown="0">
+  <autoFilter ref="E1:G37" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7A239594-29E1-43D2-A7C7-BAD18B95F548}" name="Name"/>
     <tableColumn id="2" xr3:uid="{88D0DB9C-FE4B-4B88-80D2-A005BCE333DB}" name="GP"/>
@@ -782,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X44"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,9 +693,6 @@
       <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -840,9 +713,6 @@
       <c r="G2">
         <v>370</v>
       </c>
-      <c r="K2" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -863,9 +733,6 @@
       <c r="G3">
         <v>410</v>
       </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -886,9 +753,6 @@
       <c r="G4">
         <v>610</v>
       </c>
-      <c r="K4" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -901,13 +765,13 @@
         <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>700</v>
+      </c>
+      <c r="G5">
+        <v>740</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -921,7 +785,7 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="F6">
         <v>165</v>
@@ -929,9 +793,7 @@
       <c r="G6">
         <v>510</v>
       </c>
-      <c r="K6" t="s">
-        <v>69</v>
-      </c>
+      <c r="L6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -956,9 +818,6 @@
       <c r="G7">
         <v>320</v>
       </c>
-      <c r="K7" t="s">
-        <v>70</v>
-      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -975,16 +834,13 @@
         <v>700</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="F8">
-        <v>125</v>
+        <v>365</v>
       </c>
       <c r="G8">
-        <v>290</v>
-      </c>
-      <c r="K8" t="s">
-        <v>71</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -998,16 +854,13 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="F9">
-        <v>365</v>
+        <v>180</v>
       </c>
       <c r="G9">
-        <v>2750</v>
-      </c>
-      <c r="K9" t="s">
-        <v>72</v>
+        <v>580</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1021,16 +874,13 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="F10">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="G10">
-        <v>580</v>
-      </c>
-      <c r="K10" t="s">
-        <v>73</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1044,13 +894,13 @@
         <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="F11">
-        <v>190</v>
+        <v>3000</v>
       </c>
       <c r="G11">
-        <v>680</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1064,22 +914,16 @@
         <v>120</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="F12">
-        <v>3000</v>
+        <v>75</v>
       </c>
       <c r="G12">
-        <v>3000</v>
+        <v>800</v>
       </c>
       <c r="H12" t="s">
-        <v>125</v>
-      </c>
-      <c r="K12" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1093,22 +937,16 @@
         <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="F13">
-        <v>75</v>
+        <v>3000</v>
       </c>
       <c r="G13">
-        <v>800</v>
+        <v>4000</v>
       </c>
       <c r="H13" t="s">
-        <v>125</v>
-      </c>
-      <c r="K13" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1122,19 +960,13 @@
         <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="F14">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="G14">
-        <v>4000</v>
-      </c>
-      <c r="K14" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>94</v>
+        <v>720</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1147,11 +979,14 @@
       <c r="C15">
         <v>90</v>
       </c>
-      <c r="K15" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>95</v>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <v>145</v>
+      </c>
+      <c r="G15">
+        <v>460</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1164,14 +999,17 @@
       <c r="C16">
         <v>120</v>
       </c>
-      <c r="K16" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16">
+        <v>350</v>
+      </c>
+      <c r="G16">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1181,14 +1019,17 @@
       <c r="C17">
         <v>140</v>
       </c>
-      <c r="K17" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17">
+        <v>300</v>
+      </c>
+      <c r="G17">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1198,14 +1039,17 @@
       <c r="C18">
         <v>1200</v>
       </c>
-      <c r="K18" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18">
+        <v>230</v>
+      </c>
+      <c r="G18">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1215,14 +1059,17 @@
       <c r="C19">
         <v>260</v>
       </c>
-      <c r="K19" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19">
+        <v>350</v>
+      </c>
+      <c r="G19">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1232,14 +1079,17 @@
       <c r="C20">
         <v>140</v>
       </c>
-      <c r="K20" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20">
+        <v>230</v>
+      </c>
+      <c r="G20">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1249,14 +1099,17 @@
       <c r="C21">
         <v>130</v>
       </c>
-      <c r="K21" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>3000</v>
+      </c>
+      <c r="G21">
+        <v>4820</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1266,8 +1119,17 @@
       <c r="C22">
         <v>400</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22">
+        <v>4000</v>
+      </c>
+      <c r="G22">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1277,11 +1139,8 @@
       <c r="C23">
         <v>160</v>
       </c>
-      <c r="K23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1291,11 +1150,8 @@
       <c r="C24">
         <v>240</v>
       </c>
-      <c r="K24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1305,11 +1161,8 @@
       <c r="C25">
         <v>190</v>
       </c>
-      <c r="K25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1319,23 +1172,8 @@
       <c r="C26">
         <v>120</v>
       </c>
-      <c r="K26" t="s">
-        <v>87</v>
-      </c>
-      <c r="S26" t="s">
-        <v>105</v>
-      </c>
-      <c r="T26" t="s">
-        <v>106</v>
-      </c>
-      <c r="W26" t="s">
-        <v>105</v>
-      </c>
-      <c r="X26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1345,25 +1183,8 @@
       <c r="C27">
         <v>240</v>
       </c>
-      <c r="K27" t="s">
-        <v>88</v>
-      </c>
-      <c r="R27" t="s">
-        <v>103</v>
-      </c>
-      <c r="V27" t="s">
-        <v>108</v>
-      </c>
-      <c r="W27">
-        <f>W30/3</f>
-        <v>125</v>
-      </c>
-      <c r="X27">
-        <f>X30/3</f>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1373,25 +1194,8 @@
       <c r="C28">
         <v>160</v>
       </c>
-      <c r="K28" t="s">
-        <v>89</v>
-      </c>
-      <c r="R28" t="s">
-        <v>104</v>
-      </c>
-      <c r="V28" t="s">
-        <v>111</v>
-      </c>
-      <c r="W28">
-        <f>F6</f>
-        <v>165</v>
-      </c>
-      <c r="X28">
-        <f>G6</f>
-        <v>510</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1401,17 +1205,8 @@
       <c r="C29">
         <v>150</v>
       </c>
-      <c r="K29" t="s">
-        <v>90</v>
-      </c>
-      <c r="W29">
-        <v>540</v>
-      </c>
-      <c r="X29">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1421,153 +1216,82 @@
       <c r="C30">
         <v>1500</v>
       </c>
-      <c r="K30" t="s">
-        <v>91</v>
-      </c>
-      <c r="W30">
-        <f>W29-W28</f>
-        <v>375</v>
-      </c>
-      <c r="X30">
-        <f>X29-X28</f>
-        <v>870</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
-      <c r="K31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>125</v>
+      </c>
+      <c r="C31">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
-      <c r="K32" t="s">
-        <v>83</v>
-      </c>
-      <c r="R32" t="s">
-        <v>108</v>
-      </c>
-      <c r="V32" t="s">
-        <v>112</v>
-      </c>
-      <c r="W32">
-        <f>F11</f>
-        <v>190</v>
-      </c>
-      <c r="X32">
-        <f>G11</f>
-        <v>680</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>125</v>
+      </c>
+      <c r="C32">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
-      <c r="R33" t="s">
-        <v>109</v>
-      </c>
-      <c r="V33" t="s">
-        <v>113</v>
-      </c>
-      <c r="W33">
-        <f>3*F10</f>
-        <v>540</v>
-      </c>
-      <c r="X33">
-        <f>3*G10</f>
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
-      <c r="R34" t="s">
-        <v>110</v>
-      </c>
-      <c r="V34">
-        <v>4</v>
-      </c>
-      <c r="W34">
-        <f>W33+W32</f>
-        <v>730</v>
-      </c>
-      <c r="X34">
-        <f>X33+X32</f>
-        <v>2420</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>120</v>
+      </c>
+      <c r="C34">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
-      <c r="V35">
-        <v>1</v>
-      </c>
-      <c r="X35">
-        <f>X34/4</f>
-        <v>605</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>80</v>
+      </c>
+      <c r="C35">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="R37" t="s">
-        <v>114</v>
-      </c>
-      <c r="V37" t="s">
-        <v>116</v>
-      </c>
-      <c r="W37">
-        <v>365</v>
-      </c>
-      <c r="X37">
-        <v>2750</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R38" t="s">
-        <v>112</v>
-      </c>
-      <c r="V38">
-        <v>4</v>
-      </c>
-      <c r="X38">
-        <f>2750/4</f>
-        <v>687.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R39" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R42" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R44" t="s">
-        <v>120</v>
+      <c r="B36">
+        <v>105</v>
+      </c>
+      <c r="C36">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A36 E2:E36">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
forgot to save latest spreadsheet
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -271,6 +271,93 @@
   </si>
   <si>
     <t>Kainazzo</t>
+  </si>
+  <si>
+    <t>Troian Landscape -005</t>
+  </si>
+  <si>
+    <t>----------------</t>
+  </si>
+  <si>
+    <t>01: 088(058): StingRat x3, Treant   x2</t>
+  </si>
+  <si>
+    <t>02: 089(059): Panther  x1, StingRat x3</t>
+  </si>
+  <si>
+    <t>03: 090(05A): Cannibal x1, Treant   x2</t>
+  </si>
+  <si>
+    <t>04: 091(05B): Python   x1, StingRat x2</t>
+  </si>
+  <si>
+    <t>05: 088(058): StingRat x3, Treant   x2</t>
+  </si>
+  <si>
+    <t>06: 089(059): Panther  x1, StingRat x3</t>
+  </si>
+  <si>
+    <t>07: 090(05A): Cannibal x1, Treant   x2</t>
+  </si>
+  <si>
+    <t>08: 091(05B): Python   x1, StingRat x2</t>
+  </si>
+  <si>
+    <t>Agart Island -006</t>
+  </si>
+  <si>
+    <t>------------</t>
+  </si>
+  <si>
+    <t>01: 136(088): Roc      x1, Roc Baby x2</t>
+  </si>
+  <si>
+    <t>02: 139(08B): HugeCell x3</t>
+  </si>
+  <si>
+    <t>03: 210(0D2): FlameDog x2, BlackLiz x2</t>
+  </si>
+  <si>
+    <t>04: 145(091): Ironback x2, BlackLiz x2</t>
+  </si>
+  <si>
+    <t>05: 137(089): Roc      x1, Roc Baby x3</t>
+  </si>
+  <si>
+    <t>06: 138(08A): HugeCell x4</t>
+  </si>
+  <si>
+    <t>07: 210(0D2): FlameDog x2, BlackLiz x2</t>
+  </si>
+  <si>
+    <t>08: 145(091): Ironback x2, BlackLiz x2</t>
+  </si>
+  <si>
+    <t>Eblan Cave Entrance -042</t>
+  </si>
+  <si>
+    <t>-------------------</t>
+  </si>
+  <si>
+    <t>01: 140(08C): GiantBat x3</t>
+  </si>
+  <si>
+    <t>02: 143(08F): Ironback x2</t>
+  </si>
+  <si>
+    <t>03: 146(092): Skull    x3</t>
+  </si>
+  <si>
+    <t>05: 147(093): Skull    x4</t>
+  </si>
+  <si>
+    <t>06: 142(08E): GiantBat x3, Cave Bat x3</t>
+  </si>
+  <si>
+    <t>07: 150(096): Staleman x1, Skull    x2</t>
+  </si>
+  <si>
+    <t>08: 149(095): Staleman x1</t>
   </si>
 </sst>
 </file>
@@ -661,7 +748,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="J23" sqref="J23:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,6 +780,9 @@
       <c r="G1" t="s">
         <v>40</v>
       </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -713,6 +803,9 @@
       <c r="G2">
         <v>370</v>
       </c>
+      <c r="J2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -733,6 +826,9 @@
       <c r="G3">
         <v>410</v>
       </c>
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -753,6 +849,9 @@
       <c r="G4">
         <v>610</v>
       </c>
+      <c r="J4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -773,6 +872,9 @@
       <c r="G5">
         <v>740</v>
       </c>
+      <c r="J5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -792,6 +894,9 @@
       </c>
       <c r="G6">
         <v>510</v>
+      </c>
+      <c r="J6" t="s">
+        <v>87</v>
       </c>
       <c r="L6" s="1"/>
       <c r="Q6" s="1"/>
@@ -818,6 +923,9 @@
       <c r="G7">
         <v>320</v>
       </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -842,6 +950,9 @@
       <c r="G8">
         <v>2750</v>
       </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -862,6 +973,9 @@
       <c r="G9">
         <v>580</v>
       </c>
+      <c r="J9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -882,6 +996,9 @@
       <c r="G10">
         <v>680</v>
       </c>
+      <c r="J10" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -925,6 +1042,9 @@
       <c r="H12" t="s">
         <v>71</v>
       </c>
+      <c r="J12" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -948,6 +1068,9 @@
       <c r="H13" t="s">
         <v>71</v>
       </c>
+      <c r="J13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -968,6 +1091,9 @@
       <c r="G14">
         <v>720</v>
       </c>
+      <c r="J14" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -988,6 +1114,9 @@
       <c r="G15">
         <v>460</v>
       </c>
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1008,8 +1137,11 @@
       <c r="G16">
         <v>1050</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1028,8 +1160,11 @@
       <c r="G17">
         <v>870</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1048,8 +1183,11 @@
       <c r="G18">
         <v>650</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1068,8 +1206,11 @@
       <c r="G19">
         <v>1200</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1088,8 +1229,11 @@
       <c r="G20">
         <v>680</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1108,8 +1252,11 @@
       <c r="G21">
         <v>4820</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1129,7 +1276,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1139,8 +1286,11 @@
       <c r="C23">
         <v>160</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1150,8 +1300,11 @@
       <c r="C24">
         <v>240</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1161,8 +1314,11 @@
       <c r="C25">
         <v>190</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1172,8 +1328,11 @@
       <c r="C26">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1183,8 +1342,11 @@
       <c r="C27">
         <v>240</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1194,8 +1356,11 @@
       <c r="C28">
         <v>160</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1205,8 +1370,11 @@
       <c r="C29">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1216,8 +1384,11 @@
       <c r="C30">
         <v>1500</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1227,8 +1398,11 @@
       <c r="C31">
         <v>240</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1237,6 +1411,9 @@
       </c>
       <c r="C32">
         <v>290</v>
+      </c>
+      <c r="J32" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
this should cover all overworld (outside) enemy data
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -273,91 +273,34 @@
     <t>Kainazzo</t>
   </si>
   <si>
-    <t>Troian Landscape -005</t>
-  </si>
-  <si>
-    <t>----------------</t>
-  </si>
-  <si>
-    <t>01: 088(058): StingRat x3, Treant   x2</t>
-  </si>
-  <si>
-    <t>02: 089(059): Panther  x1, StingRat x3</t>
-  </si>
-  <si>
-    <t>03: 090(05A): Cannibal x1, Treant   x2</t>
-  </si>
-  <si>
-    <t>04: 091(05B): Python   x1, StingRat x2</t>
-  </si>
-  <si>
-    <t>05: 088(058): StingRat x3, Treant   x2</t>
-  </si>
-  <si>
-    <t>06: 089(059): Panther  x1, StingRat x3</t>
-  </si>
-  <si>
-    <t>07: 090(05A): Cannibal x1, Treant   x2</t>
-  </si>
-  <si>
-    <t>08: 091(05B): Python   x1, StingRat x2</t>
-  </si>
-  <si>
-    <t>Agart Island -006</t>
-  </si>
-  <si>
-    <t>------------</t>
-  </si>
-  <si>
-    <t>01: 136(088): Roc      x1, Roc Baby x2</t>
-  </si>
-  <si>
-    <t>02: 139(08B): HugeCell x3</t>
-  </si>
-  <si>
-    <t>03: 210(0D2): FlameDog x2, BlackLiz x2</t>
-  </si>
-  <si>
-    <t>04: 145(091): Ironback x2, BlackLiz x2</t>
-  </si>
-  <si>
-    <t>05: 137(089): Roc      x1, Roc Baby x3</t>
-  </si>
-  <si>
-    <t>06: 138(08A): HugeCell x4</t>
-  </si>
-  <si>
-    <t>07: 210(0D2): FlameDog x2, BlackLiz x2</t>
-  </si>
-  <si>
-    <t>08: 145(091): Ironback x2, BlackLiz x2</t>
-  </si>
-  <si>
-    <t>Eblan Cave Entrance -042</t>
-  </si>
-  <si>
-    <t>-------------------</t>
-  </si>
-  <si>
-    <t>01: 140(08C): GiantBat x3</t>
-  </si>
-  <si>
-    <t>02: 143(08F): Ironback x2</t>
-  </si>
-  <si>
-    <t>03: 146(092): Skull    x3</t>
-  </si>
-  <si>
-    <t>05: 147(093): Skull    x4</t>
-  </si>
-  <si>
-    <t>06: 142(08E): GiantBat x3, Cave Bat x3</t>
-  </si>
-  <si>
-    <t>07: 150(096): Staleman x1, Skull    x2</t>
-  </si>
-  <si>
-    <t>08: 149(095): Staleman x1</t>
+    <t>StingRat</t>
+  </si>
+  <si>
+    <t>Treant</t>
+  </si>
+  <si>
+    <t>Panther</t>
+  </si>
+  <si>
+    <t>Cannibal</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Roc</t>
+  </si>
+  <si>
+    <t>Roc Baby</t>
+  </si>
+  <si>
+    <t>HugeCell</t>
+  </si>
+  <si>
+    <t>FlameDog</t>
+  </si>
+  <si>
+    <t>BlackLiz</t>
   </si>
 </sst>
 </file>
@@ -437,8 +380,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G37" totalsRowShown="0">
-  <autoFilter ref="E1:G37" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G36" totalsRowShown="0">
+  <autoFilter ref="E1:G36" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7A239594-29E1-43D2-A7C7-BAD18B95F548}" name="Name"/>
     <tableColumn id="2" xr3:uid="{88D0DB9C-FE4B-4B88-80D2-A005BCE333DB}" name="GP"/>
@@ -748,7 +691,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23:J32"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,9 +723,6 @@
       <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -803,9 +743,6 @@
       <c r="G2">
         <v>370</v>
       </c>
-      <c r="J2" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -826,9 +763,6 @@
       <c r="G3">
         <v>410</v>
       </c>
-      <c r="J3" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -849,9 +783,6 @@
       <c r="G4">
         <v>610</v>
       </c>
-      <c r="J4" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -872,9 +803,6 @@
       <c r="G5">
         <v>740</v>
       </c>
-      <c r="J5" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -894,9 +822,6 @@
       </c>
       <c r="G6">
         <v>510</v>
-      </c>
-      <c r="J6" t="s">
-        <v>87</v>
       </c>
       <c r="L6" s="1"/>
       <c r="Q6" s="1"/>
@@ -923,9 +848,6 @@
       <c r="G7">
         <v>320</v>
       </c>
-      <c r="J7" t="s">
-        <v>88</v>
-      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -950,9 +872,6 @@
       <c r="G8">
         <v>2750</v>
       </c>
-      <c r="J8" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -973,9 +892,6 @@
       <c r="G9">
         <v>580</v>
       </c>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -996,9 +912,6 @@
       <c r="G10">
         <v>680</v>
       </c>
-      <c r="J10" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1042,9 +955,6 @@
       <c r="H12" t="s">
         <v>71</v>
       </c>
-      <c r="J12" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1068,9 +978,6 @@
       <c r="H13" t="s">
         <v>71</v>
       </c>
-      <c r="J13" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1091,9 +998,6 @@
       <c r="G14">
         <v>720</v>
       </c>
-      <c r="J14" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1114,9 +1018,6 @@
       <c r="G15">
         <v>460</v>
       </c>
-      <c r="J15" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1137,11 +1038,8 @@
       <c r="G16">
         <v>1050</v>
       </c>
-      <c r="J16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1160,11 +1058,8 @@
       <c r="G17">
         <v>870</v>
       </c>
-      <c r="J17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1183,11 +1078,8 @@
       <c r="G18">
         <v>650</v>
       </c>
-      <c r="J18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1206,11 +1098,8 @@
       <c r="G19">
         <v>1200</v>
       </c>
-      <c r="J19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1229,11 +1118,8 @@
       <c r="G20">
         <v>680</v>
       </c>
-      <c r="J20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1252,11 +1138,8 @@
       <c r="G21">
         <v>4820</v>
       </c>
-      <c r="J21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1276,7 +1159,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1286,11 +1169,17 @@
       <c r="C23">
         <v>160</v>
       </c>
-      <c r="J23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23">
+        <v>220</v>
+      </c>
+      <c r="G23">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1300,11 +1189,17 @@
       <c r="C24">
         <v>240</v>
       </c>
-      <c r="J24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24">
+        <v>150</v>
+      </c>
+      <c r="G24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1314,11 +1209,17 @@
       <c r="C25">
         <v>190</v>
       </c>
-      <c r="J25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25">
+        <v>255</v>
+      </c>
+      <c r="G25">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1328,11 +1229,17 @@
       <c r="C26">
         <v>120</v>
       </c>
-      <c r="J26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26">
+        <v>220</v>
+      </c>
+      <c r="G26">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1342,11 +1249,17 @@
       <c r="C27">
         <v>240</v>
       </c>
-      <c r="J27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27">
+        <v>225</v>
+      </c>
+      <c r="G27">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1356,11 +1269,17 @@
       <c r="C28">
         <v>160</v>
       </c>
-      <c r="J28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28">
+        <v>150</v>
+      </c>
+      <c r="G28">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1370,11 +1289,17 @@
       <c r="C29">
         <v>150</v>
       </c>
-      <c r="J29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29">
+        <v>85</v>
+      </c>
+      <c r="G29">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1384,11 +1309,17 @@
       <c r="C30">
         <v>1500</v>
       </c>
-      <c r="J30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30">
+        <v>255</v>
+      </c>
+      <c r="G30">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1398,11 +1329,17 @@
       <c r="C31">
         <v>240</v>
       </c>
-      <c r="J31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31">
+        <v>245</v>
+      </c>
+      <c r="G31">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1412,8 +1349,14 @@
       <c r="C32">
         <v>290</v>
       </c>
-      <c r="J32" t="s">
-        <v>110</v>
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32">
+        <v>45</v>
+      </c>
+      <c r="G32">
+        <v>1300</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
increased capture offset by 1 for both X and Y to reliably capture Cal (Brena/Calbrena) data collection through Tower of Zot minor tweak to remove spaces from existing capture data (stripped anyway on load) fixed bug that added space in some match strings after load increased X coordinate capture threshold from 1000 to 1500 added todo.txt; will look at using mouse to drag capture window
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="113">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -216,9 +216,6 @@
     <t>General</t>
   </si>
   <si>
-    <t>Dragoon appears</t>
-  </si>
-  <si>
     <t>Raven</t>
   </si>
   <si>
@@ -301,13 +298,79 @@
   </si>
   <si>
     <t>BlackLiz</t>
+  </si>
+  <si>
+    <t>Ogre</t>
+  </si>
+  <si>
+    <t>Cave Bat</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>CaveNaga</t>
+  </si>
+  <si>
+    <t>VampGirl</t>
+  </si>
+  <si>
+    <t>Dark Elf</t>
+  </si>
+  <si>
+    <t>Dragoon</t>
+  </si>
+  <si>
+    <t>IceBeast</t>
+  </si>
+  <si>
+    <t>Centaur</t>
+  </si>
+  <si>
+    <t>Carapace</t>
+  </si>
+  <si>
+    <t>Ice Liz</t>
+  </si>
+  <si>
+    <t>Gremlin</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Puppet</t>
+  </si>
+  <si>
+    <t>Slime</t>
+  </si>
+  <si>
+    <t>SwordMan</t>
+  </si>
+  <si>
+    <t>Witch</t>
+  </si>
+  <si>
+    <t>EpeeGirl</t>
+  </si>
+  <si>
+    <t>Sandy</t>
+  </si>
+  <si>
+    <t>Cindy</t>
+  </si>
+  <si>
+    <t>Mindy</t>
+  </si>
+  <si>
+    <t>Valvalis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,16 +378,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -332,18 +409,129 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -368,8 +556,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C36" totalsRowShown="0">
-  <autoFilter ref="A1:C36" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0">
+  <autoFilter ref="A1:C38" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92B7C1DE-0885-429F-9F5C-CD5B673ABB7F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4EFBCB72-C5CC-4F4D-973E-B96095039970}" name="GP"/>
@@ -380,12 +568,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G36" totalsRowShown="0">
-  <autoFilter ref="E1:G36" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G38" totalsRowShown="0">
+  <autoFilter ref="E1:G38" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7A239594-29E1-43D2-A7C7-BAD18B95F548}" name="Name"/>
     <tableColumn id="2" xr3:uid="{88D0DB9C-FE4B-4B88-80D2-A005BCE333DB}" name="GP"/>
     <tableColumn id="3" xr3:uid="{2B5D719C-C423-461E-AF1F-B7F661772F51}" name="Experience"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K38" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="I1:K38" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C525D014-8E05-4793-8C6B-F0E748D5A90D}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{3DE60367-455D-4CC0-8EA7-7199578C8493}" name="GP"/>
+    <tableColumn id="3" xr3:uid="{08283C8B-F276-4B9C-A5E5-451F4636CCA6}" name="Experience"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -688,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,9 +902,10 @@
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -723,8 +924,17 @@
       <c r="G1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -735,16 +945,25 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2">
+        <v>280</v>
+      </c>
+      <c r="K2">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -755,16 +974,25 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="G3">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>610</v>
+      </c>
+      <c r="I3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3">
+        <v>175</v>
+      </c>
+      <c r="K3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -775,16 +1003,25 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>155</v>
+        <v>700</v>
       </c>
       <c r="G4">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>740</v>
+      </c>
+      <c r="I4" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>230</v>
+      </c>
+      <c r="K4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -798,13 +1035,22 @@
         <v>64</v>
       </c>
       <c r="F5">
-        <v>700</v>
+        <v>165</v>
       </c>
       <c r="G5">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5">
+        <v>290</v>
+      </c>
+      <c r="K5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -815,21 +1061,25 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F6">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G6">
-        <v>510</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="I6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6">
+        <v>275</v>
+      </c>
+      <c r="K6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -840,20 +1090,25 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F7">
-        <v>170</v>
+        <v>365</v>
       </c>
       <c r="G7">
-        <v>320</v>
-      </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>2750</v>
+      </c>
+      <c r="I7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7">
+        <v>195</v>
+      </c>
+      <c r="K7">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -867,13 +1122,22 @@
         <v>66</v>
       </c>
       <c r="F8">
-        <v>365</v>
+        <v>180</v>
       </c>
       <c r="G8">
-        <v>2750</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8">
+        <v>180</v>
+      </c>
+      <c r="K8">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -887,13 +1151,22 @@
         <v>67</v>
       </c>
       <c r="F9">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="G9">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>680</v>
+      </c>
+      <c r="I9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -907,13 +1180,22 @@
         <v>68</v>
       </c>
       <c r="F10">
-        <v>190</v>
+        <v>3000</v>
       </c>
       <c r="G10">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J10">
+        <v>175</v>
+      </c>
+      <c r="K10">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -927,13 +1209,22 @@
         <v>69</v>
       </c>
       <c r="F11">
-        <v>3000</v>
+        <v>75</v>
       </c>
       <c r="G11">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>800</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11">
+        <v>330</v>
+      </c>
+      <c r="K11">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -944,19 +1235,28 @@
         <v>120</v>
       </c>
       <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12">
+        <v>3000</v>
+      </c>
+      <c r="G12">
+        <v>4000</v>
+      </c>
+      <c r="H12" t="s">
         <v>70</v>
       </c>
-      <c r="F12">
-        <v>75</v>
-      </c>
-      <c r="G12">
-        <v>800</v>
-      </c>
-      <c r="H12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12">
+        <v>200</v>
+      </c>
+      <c r="K12">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -970,16 +1270,25 @@
         <v>72</v>
       </c>
       <c r="F13">
+        <v>500</v>
+      </c>
+      <c r="G13">
+        <v>720</v>
+      </c>
+      <c r="H13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13">
         <v>3000</v>
       </c>
-      <c r="G13">
-        <v>4000</v>
-      </c>
-      <c r="H13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -993,13 +1302,22 @@
         <v>73</v>
       </c>
       <c r="F14">
-        <v>500</v>
+        <v>145</v>
       </c>
       <c r="G14">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+      <c r="I14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14">
+        <v>3000</v>
+      </c>
+      <c r="K14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1013,13 +1331,22 @@
         <v>74</v>
       </c>
       <c r="F15">
-        <v>145</v>
+        <v>350</v>
       </c>
       <c r="G15">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>1050</v>
+      </c>
+      <c r="I15" t="s">
+        <v>111</v>
+      </c>
+      <c r="J15">
+        <v>3000</v>
+      </c>
+      <c r="K15">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1033,10 +1360,19 @@
         <v>75</v>
       </c>
       <c r="F16">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="G16">
-        <v>1050</v>
+        <v>870</v>
+      </c>
+      <c r="I16" t="s">
+        <v>112</v>
+      </c>
+      <c r="J16">
+        <v>5500</v>
+      </c>
+      <c r="K16">
+        <v>9500</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,10 +1389,10 @@
         <v>76</v>
       </c>
       <c r="F17">
-        <v>300</v>
+        <v>230</v>
       </c>
       <c r="G17">
-        <v>870</v>
+        <v>650</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1073,10 +1409,10 @@
         <v>77</v>
       </c>
       <c r="F18">
-        <v>230</v>
+        <v>350</v>
       </c>
       <c r="G18">
-        <v>650</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,10 +1429,10 @@
         <v>78</v>
       </c>
       <c r="F19">
-        <v>350</v>
+        <v>230</v>
       </c>
       <c r="G19">
-        <v>1200</v>
+        <v>680</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,10 +1449,10 @@
         <v>79</v>
       </c>
       <c r="F20">
-        <v>230</v>
+        <v>3000</v>
       </c>
       <c r="G20">
-        <v>680</v>
+        <v>4820</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1133,10 +1469,10 @@
         <v>80</v>
       </c>
       <c r="F21">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="G21">
-        <v>4820</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1153,10 +1489,10 @@
         <v>81</v>
       </c>
       <c r="F22">
-        <v>4000</v>
+        <v>220</v>
       </c>
       <c r="G22">
-        <v>5500</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,10 +1509,10 @@
         <v>82</v>
       </c>
       <c r="F23">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="G23">
-        <v>1210</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1193,10 +1529,10 @@
         <v>83</v>
       </c>
       <c r="F24">
-        <v>150</v>
+        <v>255</v>
       </c>
       <c r="G24">
-        <v>1000</v>
+        <v>830</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,10 +1549,10 @@
         <v>84</v>
       </c>
       <c r="F25">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="G25">
-        <v>830</v>
+        <v>960</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1233,10 +1569,10 @@
         <v>85</v>
       </c>
       <c r="F26">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="G26">
-        <v>960</v>
+        <v>760</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1253,10 +1589,10 @@
         <v>86</v>
       </c>
       <c r="F27">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="G27">
-        <v>760</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1273,10 +1609,10 @@
         <v>87</v>
       </c>
       <c r="F28">
-        <v>150</v>
+        <v>85</v>
       </c>
       <c r="G28">
-        <v>1410</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1293,10 +1629,10 @@
         <v>88</v>
       </c>
       <c r="F29">
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="G29">
-        <v>1010</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1313,10 +1649,10 @@
         <v>89</v>
       </c>
       <c r="F30">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="G30">
-        <v>1510</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,10 +1669,10 @@
         <v>90</v>
       </c>
       <c r="F31">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="G31">
-        <v>1720</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1353,13 +1689,13 @@
         <v>91</v>
       </c>
       <c r="F32">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="G32">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1369,8 +1705,17 @@
       <c r="C33">
         <v>320</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33">
+        <v>155</v>
+      </c>
+      <c r="G33">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1380,8 +1725,17 @@
       <c r="C34">
         <v>280</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34">
+        <v>235</v>
+      </c>
+      <c r="G34">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1391,8 +1745,17 @@
       <c r="C35">
         <v>370</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35">
+        <v>205</v>
+      </c>
+      <c r="G35">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1402,20 +1765,56 @@
       <c r="C36">
         <v>450</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36">
+        <v>195</v>
+      </c>
+      <c r="G36">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37">
+        <v>55</v>
+      </c>
+      <c r="C37">
+        <v>370</v>
+      </c>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37">
+        <v>5000</v>
+      </c>
+      <c r="G37">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A36 E2:E36">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A37:A38">
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E38 A2:A38 I20:I38 I2:I12">
+    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added bit to skip parsing if enemy roster is already full updated enemy data up to first visit to tower of bab-il
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="185">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -364,6 +364,222 @@
   </si>
   <si>
     <t>Valvalis</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Brena</t>
+  </si>
+  <si>
+    <t>Calbrena</t>
+  </si>
+  <si>
+    <t>Golbez</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Underground2 -008</t>
+  </si>
+  <si>
+    <t>------------</t>
+  </si>
+  <si>
+    <t>01: 314(13A): TrapRose x2</t>
+  </si>
+  <si>
+    <t>02: 315(13B): RocLarva x4</t>
+  </si>
+  <si>
+    <t>03: 316(13C): RockMoth x2</t>
+  </si>
+  <si>
+    <t>04: 317(13D): RockMoth x2, RocLarva x2</t>
+  </si>
+  <si>
+    <t>05: 318(13E): TrapRose x1, RockMoth x2</t>
+  </si>
+  <si>
+    <t>06: 319(13F): TrapRose x1, RockMoth x2, RocLarva x2</t>
+  </si>
+  <si>
+    <t>07: 313(139): TrapRose x1, Centpede x2</t>
+  </si>
+  <si>
+    <t>08: 312(138): Centpede x1</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 1 -044</t>
+  </si>
+  <si>
+    <t>-----------------------</t>
+  </si>
+  <si>
+    <t>01: 269(10D): Marion   x1, (Summon EvilDoll x1), EvilDoll x2</t>
+  </si>
+  <si>
+    <t>02: 265(109): Marion   x1, (Summon EvilDoll x1), EvilDoll x3</t>
+  </si>
+  <si>
+    <t>03: 261(105): Tortoise x1,  Dark Imp        x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 2 -045</t>
+  </si>
+  <si>
+    <t>03: 269(10D): FlameMan x1,  FlameDog        x2</t>
+  </si>
+  <si>
+    <t>04: 270(10E): FlameMan x2,  FlameDog        x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 3 -046</t>
+  </si>
+  <si>
+    <t>01: 269(10D): FlameMan     x1, FlameDog x2</t>
+  </si>
+  <si>
+    <t>04: 273(111): Egg(BlackLiz x1)</t>
+  </si>
+  <si>
+    <t>08: 277(115): Tofu         x6</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 4 -047</t>
+  </si>
+  <si>
+    <t>01: 273(111): Egg(BlackLiz x1)</t>
+  </si>
+  <si>
+    <t>04: 278(116): Chimera      x1, Tofu     x3</t>
+  </si>
+  <si>
+    <t>05: 279(117): Chimera      x1</t>
+  </si>
+  <si>
+    <t>06: 280(118): Chimera      x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 5 -048</t>
+  </si>
+  <si>
+    <t>01: 278(116): Chimera  x1, Tofu     x3</t>
+  </si>
+  <si>
+    <t>02: 279(117): Chimera  x1</t>
+  </si>
+  <si>
+    <t>03: 280(118): Chimera  x2</t>
+  </si>
+  <si>
+    <t>04: 281(119): Chimera  x1, FlameMan x1</t>
+  </si>
+  <si>
+    <t>05: 282(11A): Chimera  x1, FlameMan x2</t>
+  </si>
+  <si>
+    <t>06: 283(11B): Chimera  x1, FlameDog x2</t>
+  </si>
+  <si>
+    <t>08: 277(115): Tofu     x6</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 6 -049</t>
+  </si>
+  <si>
+    <t>01: 289(121): Alert    x1, (Summon Naga     x1)</t>
+  </si>
+  <si>
+    <t>02: 290(122): Alert    x1, (Summon FlameDog x1)</t>
+  </si>
+  <si>
+    <t>04: 284(11C): Stoneman x1,  Medusa          x1</t>
+  </si>
+  <si>
+    <t>05: 283(11B): Chimera  x1,  FlameDog        x2</t>
+  </si>
+  <si>
+    <t>06: 285(11D): Medusa   x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 7 -050</t>
+  </si>
+  <si>
+    <t>01: 284(11C): Stoneman x1,  Medusa          x1</t>
+  </si>
+  <si>
+    <t>02: 285(11D): Medusa   x2</t>
+  </si>
+  <si>
+    <t>03: 289(121): Alert    x1, (Summon Naga     x1)</t>
+  </si>
+  <si>
+    <t>04: 290(122): Alert    x1, (Summon FlameDog x1)</t>
+  </si>
+  <si>
+    <t>05: 286(11E): Stoneman x2</t>
+  </si>
+  <si>
+    <t>06: 287(11F): Alert    x1, (Summon Chimera  x1)</t>
+  </si>
+  <si>
+    <t>07: 277(115): Tofu     x6</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Floor 8 -051</t>
+  </si>
+  <si>
+    <t>02: 283(11B): Chimera  x1,  FlameDog        x2</t>
+  </si>
+  <si>
+    <t>04: 286(11E): Stoneman x2</t>
+  </si>
+  <si>
+    <t>05: 288(120): Alert    x1, (Summon Stoneman x1)</t>
+  </si>
+  <si>
+    <t>07: 276(114): Tofu     x4</t>
+  </si>
+  <si>
+    <t>08: 280(118): Chimera  x2</t>
+  </si>
+  <si>
+    <t>Armadilo</t>
+  </si>
+  <si>
+    <t>Tortoise</t>
+  </si>
+  <si>
+    <t>Dark Imp</t>
+  </si>
+  <si>
+    <t>FlameMan</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Tofu</t>
+  </si>
+  <si>
+    <t>EvilDoll</t>
+  </si>
+  <si>
+    <t>Chimera</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>Naga</t>
+  </si>
+  <si>
+    <t>Stoneman</t>
+  </si>
+  <si>
+    <t>Medusa</t>
   </si>
 </sst>
 </file>
@@ -453,7 +669,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -509,26 +725,6 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -888,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +1101,7 @@
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -933,8 +1129,14 @@
       <c r="K1" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -962,8 +1164,14 @@
       <c r="K2">
         <v>1570</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>119</v>
+      </c>
+      <c r="S2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -991,8 +1199,14 @@
       <c r="K3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>120</v>
+      </c>
+      <c r="S3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1020,8 +1234,14 @@
       <c r="K4">
         <v>1350</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>121</v>
+      </c>
+      <c r="S4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1049,8 +1269,14 @@
       <c r="K5">
         <v>1500</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>122</v>
+      </c>
+      <c r="S5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1078,8 +1304,14 @@
       <c r="K6">
         <v>1500</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>123</v>
+      </c>
+      <c r="S6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1107,8 +1339,14 @@
       <c r="K7">
         <v>1110</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>124</v>
+      </c>
+      <c r="S7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1136,8 +1374,14 @@
       <c r="K8">
         <v>950</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>125</v>
+      </c>
+      <c r="S8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1165,8 +1409,14 @@
       <c r="K9">
         <v>760</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>126</v>
+      </c>
+      <c r="S9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1194,8 +1444,11 @@
       <c r="K10">
         <v>1100</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1223,8 +1476,11 @@
       <c r="K11">
         <v>1670</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1255,8 +1511,14 @@
       <c r="K12">
         <v>1260</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>128</v>
+      </c>
+      <c r="S12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1287,8 +1549,14 @@
       <c r="K13">
         <v>3000</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>129</v>
+      </c>
+      <c r="S13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1316,8 +1584,14 @@
       <c r="K14">
         <v>3000</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>130</v>
+      </c>
+      <c r="S14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1345,8 +1619,14 @@
       <c r="K15">
         <v>3000</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>131</v>
+      </c>
+      <c r="S15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1374,8 +1654,14 @@
       <c r="K16">
         <v>9500</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>132</v>
+      </c>
+      <c r="S16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1394,8 +1680,20 @@
       <c r="G17">
         <v>650</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17">
+        <v>500</v>
+      </c>
+      <c r="K17">
+        <v>1000</v>
+      </c>
+      <c r="S17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1414,8 +1712,23 @@
       <c r="G18">
         <v>1200</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18">
+        <v>500</v>
+      </c>
+      <c r="K18">
+        <v>1000</v>
+      </c>
+      <c r="M18" t="s">
+        <v>133</v>
+      </c>
+      <c r="S18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1434,8 +1747,23 @@
       <c r="G19">
         <v>680</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19">
+        <v>6500</v>
+      </c>
+      <c r="K19">
+        <v>18000</v>
+      </c>
+      <c r="M19" t="s">
+        <v>129</v>
+      </c>
+      <c r="S19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1454,8 +1782,20 @@
       <c r="G20">
         <v>4820</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20">
+        <v>11000</v>
+      </c>
+      <c r="K20">
+        <v>20000</v>
+      </c>
+      <c r="M20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1474,8 +1814,23 @@
       <c r="G21">
         <v>5500</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>134</v>
+      </c>
+      <c r="S21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1494,8 +1849,23 @@
       <c r="G22">
         <v>1210</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>173</v>
+      </c>
+      <c r="J22">
+        <v>195</v>
+      </c>
+      <c r="K22">
+        <v>1600</v>
+      </c>
+      <c r="M22" t="s">
+        <v>135</v>
+      </c>
+      <c r="S22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1514,8 +1884,20 @@
       <c r="G23">
         <v>1000</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23">
+        <v>235</v>
+      </c>
+      <c r="K23">
+        <v>1700</v>
+      </c>
+      <c r="S23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1534,8 +1916,23 @@
       <c r="G24">
         <v>830</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>175</v>
+      </c>
+      <c r="J24">
+        <v>45</v>
+      </c>
+      <c r="K24">
+        <v>1940</v>
+      </c>
+      <c r="M24" t="s">
+        <v>136</v>
+      </c>
+      <c r="S24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1554,8 +1951,17 @@
       <c r="G25">
         <v>960</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>176</v>
+      </c>
+      <c r="M25" t="s">
+        <v>129</v>
+      </c>
+      <c r="S25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1574,8 +1980,17 @@
       <c r="G26">
         <v>760</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>177</v>
+      </c>
+      <c r="M26" t="s">
+        <v>137</v>
+      </c>
+      <c r="S26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1594,8 +2009,17 @@
       <c r="G27">
         <v>1410</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>178</v>
+      </c>
+      <c r="M27" t="s">
+        <v>138</v>
+      </c>
+      <c r="S27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1614,8 +2038,17 @@
       <c r="G28">
         <v>1010</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>179</v>
+      </c>
+      <c r="M28" t="s">
+        <v>139</v>
+      </c>
+      <c r="S28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1634,8 +2067,14 @@
       <c r="G29">
         <v>1510</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>180</v>
+      </c>
+      <c r="S29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1654,8 +2093,17 @@
       <c r="G30">
         <v>1720</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>181</v>
+      </c>
+      <c r="M30" t="s">
+        <v>140</v>
+      </c>
+      <c r="S30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1674,8 +2122,14 @@
       <c r="G31">
         <v>1300</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1694,8 +2148,17 @@
       <c r="G32">
         <v>1100</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>183</v>
+      </c>
+      <c r="M32" t="s">
+        <v>141</v>
+      </c>
+      <c r="S32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1714,8 +2177,17 @@
       <c r="G33">
         <v>630</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>184</v>
+      </c>
+      <c r="M33" t="s">
+        <v>142</v>
+      </c>
+      <c r="S33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1734,8 +2206,14 @@
       <c r="G34">
         <v>1100</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>143</v>
+      </c>
+      <c r="S34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1754,8 +2232,14 @@
       <c r="G35">
         <v>750</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>144</v>
+      </c>
+      <c r="S35" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1774,8 +2258,14 @@
       <c r="G36">
         <v>820</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>139</v>
+      </c>
+      <c r="S36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -1794,21 +2284,48 @@
       <c r="G37">
         <v>6000</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="S37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
       <c r="D38" t="s">
         <v>70</v>
       </c>
+      <c r="S38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S41" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A37:A38">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E38 A2:A38 I20:I38 I2:I12">
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">

</xml_diff>

<commit_message>
completed data collection through Eblan cave added edge case for Lugae/Lugaeborg; since both are named Dr.Lugae, I might change the name of Lugaeborg back
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="177">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -411,141 +411,6 @@
     <t>08: 312(138): Centpede x1</t>
   </si>
   <si>
-    <t>Tower of Bab-il Floor 1 -044</t>
-  </si>
-  <si>
-    <t>-----------------------</t>
-  </si>
-  <si>
-    <t>01: 269(10D): Marion   x1, (Summon EvilDoll x1), EvilDoll x2</t>
-  </si>
-  <si>
-    <t>02: 265(109): Marion   x1, (Summon EvilDoll x1), EvilDoll x3</t>
-  </si>
-  <si>
-    <t>03: 261(105): Tortoise x1,  Dark Imp        x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 2 -045</t>
-  </si>
-  <si>
-    <t>03: 269(10D): FlameMan x1,  FlameDog        x2</t>
-  </si>
-  <si>
-    <t>04: 270(10E): FlameMan x2,  FlameDog        x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 3 -046</t>
-  </si>
-  <si>
-    <t>01: 269(10D): FlameMan     x1, FlameDog x2</t>
-  </si>
-  <si>
-    <t>04: 273(111): Egg(BlackLiz x1)</t>
-  </si>
-  <si>
-    <t>08: 277(115): Tofu         x6</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 4 -047</t>
-  </si>
-  <si>
-    <t>01: 273(111): Egg(BlackLiz x1)</t>
-  </si>
-  <si>
-    <t>04: 278(116): Chimera      x1, Tofu     x3</t>
-  </si>
-  <si>
-    <t>05: 279(117): Chimera      x1</t>
-  </si>
-  <si>
-    <t>06: 280(118): Chimera      x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 5 -048</t>
-  </si>
-  <si>
-    <t>01: 278(116): Chimera  x1, Tofu     x3</t>
-  </si>
-  <si>
-    <t>02: 279(117): Chimera  x1</t>
-  </si>
-  <si>
-    <t>03: 280(118): Chimera  x2</t>
-  </si>
-  <si>
-    <t>04: 281(119): Chimera  x1, FlameMan x1</t>
-  </si>
-  <si>
-    <t>05: 282(11A): Chimera  x1, FlameMan x2</t>
-  </si>
-  <si>
-    <t>06: 283(11B): Chimera  x1, FlameDog x2</t>
-  </si>
-  <si>
-    <t>08: 277(115): Tofu     x6</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 6 -049</t>
-  </si>
-  <si>
-    <t>01: 289(121): Alert    x1, (Summon Naga     x1)</t>
-  </si>
-  <si>
-    <t>02: 290(122): Alert    x1, (Summon FlameDog x1)</t>
-  </si>
-  <si>
-    <t>04: 284(11C): Stoneman x1,  Medusa          x1</t>
-  </si>
-  <si>
-    <t>05: 283(11B): Chimera  x1,  FlameDog        x2</t>
-  </si>
-  <si>
-    <t>06: 285(11D): Medusa   x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 7 -050</t>
-  </si>
-  <si>
-    <t>01: 284(11C): Stoneman x1,  Medusa          x1</t>
-  </si>
-  <si>
-    <t>02: 285(11D): Medusa   x2</t>
-  </si>
-  <si>
-    <t>03: 289(121): Alert    x1, (Summon Naga     x1)</t>
-  </si>
-  <si>
-    <t>04: 290(122): Alert    x1, (Summon FlameDog x1)</t>
-  </si>
-  <si>
-    <t>05: 286(11E): Stoneman x2</t>
-  </si>
-  <si>
-    <t>06: 287(11F): Alert    x1, (Summon Chimera  x1)</t>
-  </si>
-  <si>
-    <t>07: 277(115): Tofu     x6</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Floor 8 -051</t>
-  </si>
-  <si>
-    <t>02: 283(11B): Chimera  x1,  FlameDog        x2</t>
-  </si>
-  <si>
-    <t>04: 286(11E): Stoneman x2</t>
-  </si>
-  <si>
-    <t>05: 288(120): Alert    x1, (Summon Stoneman x1)</t>
-  </si>
-  <si>
-    <t>07: 276(114): Tofu     x4</t>
-  </si>
-  <si>
-    <t>08: 280(118): Chimera  x2</t>
-  </si>
-  <si>
     <t>Armadilo</t>
   </si>
   <si>
@@ -580,6 +445,117 @@
   </si>
   <si>
     <t>Medusa</t>
+  </si>
+  <si>
+    <t>Dr.Lugae</t>
+  </si>
+  <si>
+    <t>Balnab</t>
+  </si>
+  <si>
+    <t>Lugaeborg</t>
+  </si>
+  <si>
+    <t>Balnab-Z</t>
+  </si>
+  <si>
+    <t>BlackCat</t>
+  </si>
+  <si>
+    <t>Lamia</t>
+  </si>
+  <si>
+    <t>Mad Ogre</t>
+  </si>
+  <si>
+    <t>Staleman</t>
+  </si>
+  <si>
+    <t>Skull</t>
+  </si>
+  <si>
+    <t>Eblan Cave Entrance -042</t>
+  </si>
+  <si>
+    <t>-------------------</t>
+  </si>
+  <si>
+    <t>01: 140(08C): GiantBat x3</t>
+  </si>
+  <si>
+    <t>02: 143(08F): Ironback x2</t>
+  </si>
+  <si>
+    <t>03: 146(092): Skull    x3</t>
+  </si>
+  <si>
+    <t>04: 145(091): Ironback x2, BlackLiz x2</t>
+  </si>
+  <si>
+    <t>05: 147(093): Skull    x4</t>
+  </si>
+  <si>
+    <t>06: 142(08E): GiantBat x3, Cave Bat x3</t>
+  </si>
+  <si>
+    <t>07: 150(096): Staleman x1, Skull    x2</t>
+  </si>
+  <si>
+    <t>08: 149(095): Staleman x1</t>
+  </si>
+  <si>
+    <t>Pass to Bab-il -043</t>
+  </si>
+  <si>
+    <t>--------------</t>
+  </si>
+  <si>
+    <t>01: 141(08D): GiantBat x4</t>
+  </si>
+  <si>
+    <t>02: 144(090): Ironback x1, Armadilo x1, BlackLiz x1</t>
+  </si>
+  <si>
+    <t>03: 147(093): Skull    x4</t>
+  </si>
+  <si>
+    <t>05: 146(092): Skull    x3</t>
+  </si>
+  <si>
+    <t>Pass to Bab-il2 -029</t>
+  </si>
+  <si>
+    <t>-----------------</t>
+  </si>
+  <si>
+    <t>01: 141(08D): GiantBat     x4</t>
+  </si>
+  <si>
+    <t>02: 144(090): Ironback     x1, Armadilo x1, BlackLiz x1</t>
+  </si>
+  <si>
+    <t>03: 148(094): Red Bone     x3, Skull    x2</t>
+  </si>
+  <si>
+    <t>04: 160(0A0): Egg(Lamia    x1)</t>
+  </si>
+  <si>
+    <t>05: 142(08E): GiantBat     x3, Cave Bat x3</t>
+  </si>
+  <si>
+    <t>06: 145(091): Ironback     x2, BlackLiz x2</t>
+  </si>
+  <si>
+    <t>07: 151(097): Staleman     x1, Skull    x2, Red Bone x2</t>
+  </si>
+  <si>
+    <t>08: 149(095): Staleman     x1</t>
+  </si>
+  <si>
+    <t>GiantBat</t>
+  </si>
+  <si>
+    <t>Ironback</t>
   </si>
 </sst>
 </file>
@@ -669,7 +645,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -738,6 +714,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -752,8 +738,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0">
-  <autoFilter ref="A1:C38" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C42" totalsRowShown="0">
+  <autoFilter ref="A1:C42" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92B7C1DE-0885-429F-9F5C-CD5B673ABB7F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4EFBCB72-C5CC-4F4D-973E-B96095039970}" name="GP"/>
@@ -764,8 +750,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G38" totalsRowShown="0">
-  <autoFilter ref="E1:G38" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G42" totalsRowShown="0">
+  <autoFilter ref="E1:G42" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7A239594-29E1-43D2-A7C7-BAD18B95F548}" name="Name"/>
     <tableColumn id="2" xr3:uid="{88D0DB9C-FE4B-4B88-80D2-A005BCE333DB}" name="GP"/>
@@ -776,8 +762,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K38" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="I1:K38" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K42" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="I1:K42" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C525D014-8E05-4793-8C6B-F0E748D5A90D}" name="Name"/>
     <tableColumn id="2" xr3:uid="{3DE60367-455D-4CC0-8EA7-7199578C8493}" name="GP"/>
@@ -1084,24 +1070,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1130,13 +1118,13 @@
         <v>40</v>
       </c>
       <c r="M1" t="s">
+        <v>149</v>
+      </c>
+      <c r="R1" t="s">
         <v>118</v>
       </c>
-      <c r="S1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1147,31 +1135,31 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="G2">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="J2">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="K2">
-        <v>1570</v>
+        <v>1670</v>
       </c>
       <c r="M2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" t="s">
         <v>119</v>
       </c>
-      <c r="S2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1182,31 +1170,31 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F3">
-        <v>155</v>
+        <v>365</v>
       </c>
       <c r="G3">
-        <v>610</v>
+        <v>2750</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="J3">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="K3">
-        <v>1000</v>
+        <v>1260</v>
       </c>
       <c r="M3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R3" t="s">
         <v>120</v>
       </c>
-      <c r="S3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1217,31 +1205,31 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F4">
-        <v>700</v>
+        <v>180</v>
       </c>
       <c r="G4">
-        <v>740</v>
+        <v>580</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="J4">
-        <v>230</v>
+        <v>3000</v>
       </c>
       <c r="K4">
-        <v>1350</v>
+        <v>3000</v>
       </c>
       <c r="M4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R4" t="s">
         <v>121</v>
       </c>
-      <c r="S4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1252,31 +1240,31 @@
         <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F5">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="G5">
-        <v>510</v>
+        <v>680</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="J5">
-        <v>290</v>
+        <v>3000</v>
       </c>
       <c r="K5">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="M5" t="s">
+        <v>153</v>
+      </c>
+      <c r="R5" t="s">
         <v>122</v>
       </c>
-      <c r="S5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1287,31 +1275,31 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F6">
-        <v>170</v>
+        <v>3000</v>
       </c>
       <c r="G6">
-        <v>320</v>
+        <v>3000</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="J6">
-        <v>275</v>
+        <v>3000</v>
       </c>
       <c r="K6">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="M6" t="s">
+        <v>154</v>
+      </c>
+      <c r="R6" t="s">
         <v>123</v>
       </c>
-      <c r="S6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1322,31 +1310,31 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F7">
-        <v>365</v>
+        <v>75</v>
       </c>
       <c r="G7">
-        <v>2750</v>
+        <v>800</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="J7">
-        <v>195</v>
+        <v>5500</v>
       </c>
       <c r="K7">
-        <v>1110</v>
+        <v>9500</v>
       </c>
       <c r="M7" t="s">
+        <v>155</v>
+      </c>
+      <c r="R7" t="s">
         <v>124</v>
       </c>
-      <c r="S7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1357,31 +1345,31 @@
         <v>700</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F8">
-        <v>180</v>
+        <v>3000</v>
       </c>
       <c r="G8">
-        <v>580</v>
+        <v>4000</v>
       </c>
       <c r="I8" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="J8">
-        <v>180</v>
+        <v>500</v>
       </c>
       <c r="K8">
-        <v>950</v>
+        <v>1000</v>
       </c>
       <c r="M8" t="s">
+        <v>156</v>
+      </c>
+      <c r="R8" t="s">
         <v>125</v>
       </c>
-      <c r="S8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1392,31 +1380,31 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F9">
-        <v>190</v>
+        <v>500</v>
       </c>
       <c r="G9">
-        <v>680</v>
+        <v>720</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="J9">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="K9">
-        <v>760</v>
+        <v>1000</v>
       </c>
       <c r="M9" t="s">
+        <v>157</v>
+      </c>
+      <c r="R9" t="s">
         <v>126</v>
       </c>
-      <c r="S9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1427,28 +1415,31 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F10">
-        <v>3000</v>
+        <v>145</v>
       </c>
       <c r="G10">
-        <v>3000</v>
+        <v>460</v>
       </c>
       <c r="I10" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="J10">
-        <v>175</v>
+        <v>6500</v>
       </c>
       <c r="K10">
-        <v>1100</v>
+        <v>18000</v>
       </c>
       <c r="M10" t="s">
+        <v>158</v>
+      </c>
+      <c r="R10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1459,28 +1450,25 @@
         <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F11">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="G11">
-        <v>800</v>
+        <v>1050</v>
       </c>
       <c r="I11" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="J11">
-        <v>330</v>
+        <v>11000</v>
       </c>
       <c r="K11">
-        <v>1670</v>
-      </c>
-      <c r="S11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1491,34 +1479,31 @@
         <v>120</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F12">
-        <v>3000</v>
+        <v>300</v>
       </c>
       <c r="G12">
-        <v>4000</v>
+        <v>870</v>
       </c>
       <c r="H12" t="s">
         <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="J12">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>1260</v>
+        <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>128</v>
-      </c>
-      <c r="S12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1529,34 +1514,31 @@
         <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F13">
-        <v>500</v>
+        <v>230</v>
       </c>
       <c r="G13">
-        <v>720</v>
+        <v>650</v>
       </c>
       <c r="H13" t="s">
         <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="J13">
-        <v>3000</v>
+        <v>195</v>
       </c>
       <c r="K13">
-        <v>3000</v>
+        <v>1600</v>
       </c>
       <c r="M13" t="s">
-        <v>129</v>
-      </c>
-      <c r="S13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1567,31 +1549,28 @@
         <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F14">
-        <v>145</v>
+        <v>350</v>
       </c>
       <c r="G14">
-        <v>460</v>
+        <v>1200</v>
       </c>
       <c r="I14" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="J14">
-        <v>3000</v>
+        <v>235</v>
       </c>
       <c r="K14">
-        <v>3000</v>
+        <v>1700</v>
       </c>
       <c r="M14" t="s">
-        <v>130</v>
-      </c>
-      <c r="S14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1602,31 +1581,28 @@
         <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F15">
-        <v>350</v>
+        <v>230</v>
       </c>
       <c r="G15">
-        <v>1050</v>
+        <v>680</v>
       </c>
       <c r="I15" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="J15">
-        <v>3000</v>
+        <v>45</v>
       </c>
       <c r="K15">
-        <v>3000</v>
+        <v>1940</v>
       </c>
       <c r="M15" t="s">
-        <v>131</v>
-      </c>
-      <c r="S15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1637,31 +1613,28 @@
         <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F16">
+        <v>3000</v>
+      </c>
+      <c r="G16">
+        <v>4820</v>
+      </c>
+      <c r="I16" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16">
         <v>300</v>
       </c>
-      <c r="G16">
-        <v>870</v>
-      </c>
-      <c r="I16" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16">
-        <v>5500</v>
-      </c>
       <c r="K16">
-        <v>9500</v>
+        <v>1720</v>
       </c>
       <c r="M16" t="s">
-        <v>132</v>
-      </c>
-      <c r="S16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1672,28 +1645,28 @@
         <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F17">
-        <v>230</v>
+        <v>4000</v>
       </c>
       <c r="G17">
-        <v>650</v>
+        <v>5500</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="J17">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>1000</v>
-      </c>
-      <c r="S17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1704,31 +1677,28 @@
         <v>1200</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F18">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="G18">
-        <v>1200</v>
+        <v>1210</v>
       </c>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="J18">
-        <v>500</v>
+        <v>385</v>
       </c>
       <c r="K18">
-        <v>1000</v>
+        <v>1060</v>
       </c>
       <c r="M18" t="s">
-        <v>133</v>
-      </c>
-      <c r="S18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1739,31 +1709,28 @@
         <v>260</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F19">
-        <v>230</v>
+        <v>150</v>
       </c>
       <c r="G19">
-        <v>680</v>
+        <v>1000</v>
       </c>
       <c r="I19" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="J19">
-        <v>6500</v>
+        <v>270</v>
       </c>
       <c r="K19">
-        <v>18000</v>
+        <v>1420</v>
       </c>
       <c r="M19" t="s">
-        <v>129</v>
-      </c>
-      <c r="S19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1774,28 +1741,28 @@
         <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F20">
-        <v>3000</v>
+        <v>255</v>
       </c>
       <c r="G20">
-        <v>4820</v>
+        <v>830</v>
       </c>
       <c r="I20" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="J20">
-        <v>11000</v>
+        <v>230</v>
       </c>
       <c r="K20">
-        <v>20000</v>
+        <v>2300</v>
       </c>
       <c r="M20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1806,31 +1773,28 @@
         <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F21">
-        <v>4000</v>
+        <v>220</v>
       </c>
       <c r="G21">
-        <v>5500</v>
+        <v>960</v>
       </c>
       <c r="I21" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="M21" t="s">
-        <v>134</v>
-      </c>
-      <c r="S21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1841,31 +1805,25 @@
         <v>400</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F22">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="G22">
-        <v>1210</v>
+        <v>760</v>
       </c>
       <c r="I22" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="J22">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="K22">
-        <v>1600</v>
-      </c>
-      <c r="M22" t="s">
-        <v>135</v>
-      </c>
-      <c r="S22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1876,28 +1834,28 @@
         <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F23">
         <v>150</v>
       </c>
       <c r="G23">
-        <v>1000</v>
+        <v>1410</v>
       </c>
       <c r="I23" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="J23">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="K23">
-        <v>1700</v>
-      </c>
-      <c r="S23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <v>2950</v>
+      </c>
+      <c r="M23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1908,31 +1866,28 @@
         <v>240</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F24">
-        <v>255</v>
+        <v>85</v>
       </c>
       <c r="G24">
-        <v>830</v>
+        <v>1010</v>
       </c>
       <c r="I24" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="J24">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="K24">
-        <v>1940</v>
+        <v>1250</v>
       </c>
       <c r="M24" t="s">
-        <v>136</v>
-      </c>
-      <c r="S24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1943,25 +1898,28 @@
         <v>190</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F25">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="G25">
-        <v>960</v>
+        <v>1510</v>
       </c>
       <c r="I25" t="s">
-        <v>176</v>
+        <v>140</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>129</v>
-      </c>
-      <c r="S25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1972,25 +1930,28 @@
         <v>120</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F26">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="G26">
-        <v>760</v>
+        <v>1720</v>
       </c>
       <c r="I26" t="s">
-        <v>177</v>
+        <v>141</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>137</v>
-      </c>
-      <c r="S26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2001,25 +1962,28 @@
         <v>240</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F27">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="G27">
-        <v>1410</v>
+        <v>1300</v>
       </c>
       <c r="I27" t="s">
-        <v>178</v>
+        <v>143</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>138</v>
-      </c>
-      <c r="S27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2030,25 +1994,28 @@
         <v>160</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F28">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G28">
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="I28" t="s">
-        <v>179</v>
+        <v>142</v>
+      </c>
+      <c r="J28">
+        <v>4000</v>
+      </c>
+      <c r="K28">
+        <v>3000</v>
       </c>
       <c r="M28" t="s">
-        <v>139</v>
-      </c>
-      <c r="S28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2059,22 +2026,28 @@
         <v>150</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F29">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="G29">
-        <v>1510</v>
+        <v>630</v>
       </c>
       <c r="I29" t="s">
-        <v>180</v>
-      </c>
-      <c r="S29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J29">
+        <v>345</v>
+      </c>
+      <c r="K29">
+        <v>2800</v>
+      </c>
+      <c r="M29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2085,25 +2058,28 @@
         <v>1500</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F30">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="G30">
-        <v>1720</v>
+        <v>1100</v>
       </c>
       <c r="I30" t="s">
-        <v>181</v>
+        <v>145</v>
+      </c>
+      <c r="J30">
+        <v>1210</v>
+      </c>
+      <c r="K30">
+        <v>2060</v>
       </c>
       <c r="M30" t="s">
-        <v>140</v>
-      </c>
-      <c r="S30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -2114,22 +2090,28 @@
         <v>240</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F31">
-        <v>45</v>
+        <v>205</v>
       </c>
       <c r="G31">
-        <v>1300</v>
+        <v>750</v>
       </c>
       <c r="I31" t="s">
-        <v>182</v>
+        <v>146</v>
+      </c>
+      <c r="J31">
+        <v>270</v>
+      </c>
+      <c r="K31">
+        <v>2370</v>
       </c>
       <c r="M31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2140,25 +2122,28 @@
         <v>290</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F32">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="G32">
-        <v>1100</v>
+        <v>820</v>
       </c>
       <c r="I32" t="s">
-        <v>183</v>
+        <v>147</v>
+      </c>
+      <c r="J32">
+        <v>445</v>
+      </c>
+      <c r="K32">
+        <v>2100</v>
       </c>
       <c r="M32" t="s">
-        <v>141</v>
-      </c>
-      <c r="S32" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2169,25 +2154,25 @@
         <v>320</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F33">
-        <v>155</v>
+        <v>5000</v>
       </c>
       <c r="G33">
-        <v>630</v>
+        <v>6000</v>
       </c>
       <c r="I33" t="s">
-        <v>184</v>
-      </c>
-      <c r="M33" t="s">
-        <v>142</v>
-      </c>
-      <c r="S33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="J33">
+        <v>120</v>
+      </c>
+      <c r="K33">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2198,22 +2183,25 @@
         <v>280</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F34">
-        <v>235</v>
+        <v>280</v>
       </c>
       <c r="G34">
-        <v>1100</v>
-      </c>
-      <c r="M34" t="s">
-        <v>143</v>
-      </c>
-      <c r="S34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1570</v>
+      </c>
+      <c r="I34" t="s">
+        <v>175</v>
+      </c>
+      <c r="J34">
+        <v>365</v>
+      </c>
+      <c r="K34">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -2224,22 +2212,25 @@
         <v>370</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F35">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="G35">
-        <v>750</v>
-      </c>
-      <c r="M35" t="s">
-        <v>144</v>
-      </c>
-      <c r="S35" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+      <c r="I35" t="s">
+        <v>176</v>
+      </c>
+      <c r="J35">
+        <v>235</v>
+      </c>
+      <c r="K35">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2250,22 +2241,27 @@
         <v>450</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F36">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="G36">
-        <v>820</v>
-      </c>
-      <c r="M36" t="s">
-        <v>139</v>
-      </c>
-      <c r="S36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1350</v>
+      </c>
+      <c r="M36">
+        <f>470+90</f>
+        <v>560</v>
+      </c>
+      <c r="N36">
+        <f>2600+2200</f>
+        <v>4800</v>
+      </c>
+      <c r="P36">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2276,19 +2272,24 @@
         <v>370</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F37">
-        <v>5000</v>
+        <v>290</v>
       </c>
       <c r="G37">
-        <v>6000</v>
-      </c>
-      <c r="S37" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1500</v>
+      </c>
+      <c r="N37">
+        <f>N36/4</f>
+        <v>1200</v>
+      </c>
+      <c r="P37">
+        <f>365*3+155*3</f>
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2298,34 +2299,102 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38" t="s">
-        <v>70</v>
-      </c>
-      <c r="S38" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S39" t="s">
+      <c r="E38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38">
+        <v>275</v>
+      </c>
+      <c r="G38">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>100</v>
+      </c>
+      <c r="C39">
+        <v>410</v>
+      </c>
+      <c r="E39" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39">
+        <v>195</v>
+      </c>
+      <c r="G39">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40">
+        <v>155</v>
+      </c>
+      <c r="C40">
+        <v>610</v>
+      </c>
+      <c r="E40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40">
+        <v>180</v>
+      </c>
+      <c r="G40">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41">
+        <v>700</v>
+      </c>
+      <c r="C41">
+        <v>740</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41">
+        <v>50</v>
+      </c>
+      <c r="G41">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42">
         <v>165</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S41" t="s">
-        <v>172</v>
+      <c r="C42">
+        <v>510</v>
+      </c>
+      <c r="E42" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42">
+        <v>175</v>
+      </c>
+      <c r="G42">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A37:A38">
     <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E38 A2:A38 I20:I38 I2:I12">
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+  <conditionalFormatting sqref="A2:A42 E2:E42 I2:I42">
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">

</xml_diff>

<commit_message>
changed dataClearThreshold to be the multiple of x and y offsets; basically, if absolutely none of the capture attempts produce data, clear everything out swallowing exception that pops up when closing the app; will look to address properly later prepared spreadsheet encounter data for bab-il revisit
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="214">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -381,36 +381,6 @@
     <t>Shadow</t>
   </si>
   <si>
-    <t>Underground2 -008</t>
-  </si>
-  <si>
-    <t>------------</t>
-  </si>
-  <si>
-    <t>01: 314(13A): TrapRose x2</t>
-  </si>
-  <si>
-    <t>02: 315(13B): RocLarva x4</t>
-  </si>
-  <si>
-    <t>03: 316(13C): RockMoth x2</t>
-  </si>
-  <si>
-    <t>04: 317(13D): RockMoth x2, RocLarva x2</t>
-  </si>
-  <si>
-    <t>05: 318(13E): TrapRose x1, RockMoth x2</t>
-  </si>
-  <si>
-    <t>06: 319(13F): TrapRose x1, RockMoth x2, RocLarva x2</t>
-  </si>
-  <si>
-    <t>07: 313(139): TrapRose x1, Centpede x2</t>
-  </si>
-  <si>
-    <t>08: 312(138): Centpede x1</t>
-  </si>
-  <si>
     <t>Armadilo</t>
   </si>
   <si>
@@ -474,88 +444,229 @@
     <t>Skull</t>
   </si>
   <si>
-    <t>Eblan Cave Entrance -042</t>
-  </si>
-  <si>
-    <t>-------------------</t>
-  </si>
-  <si>
-    <t>01: 140(08C): GiantBat x3</t>
-  </si>
-  <si>
-    <t>02: 143(08F): Ironback x2</t>
-  </si>
-  <si>
-    <t>03: 146(092): Skull    x3</t>
-  </si>
-  <si>
-    <t>04: 145(091): Ironback x2, BlackLiz x2</t>
-  </si>
-  <si>
-    <t>05: 147(093): Skull    x4</t>
-  </si>
-  <si>
-    <t>06: 142(08E): GiantBat x3, Cave Bat x3</t>
-  </si>
-  <si>
-    <t>07: 150(096): Staleman x1, Skull    x2</t>
-  </si>
-  <si>
-    <t>08: 149(095): Staleman x1</t>
-  </si>
-  <si>
-    <t>Pass to Bab-il -043</t>
-  </si>
-  <si>
-    <t>--------------</t>
-  </si>
-  <si>
-    <t>01: 141(08D): GiantBat x4</t>
-  </si>
-  <si>
-    <t>02: 144(090): Ironback x1, Armadilo x1, BlackLiz x1</t>
-  </si>
-  <si>
-    <t>03: 147(093): Skull    x4</t>
-  </si>
-  <si>
-    <t>05: 146(092): Skull    x3</t>
-  </si>
-  <si>
-    <t>Pass to Bab-il2 -029</t>
-  </si>
-  <si>
-    <t>-----------------</t>
-  </si>
-  <si>
-    <t>01: 141(08D): GiantBat     x4</t>
-  </si>
-  <si>
-    <t>02: 144(090): Ironback     x1, Armadilo x1, BlackLiz x1</t>
-  </si>
-  <si>
-    <t>03: 148(094): Red Bone     x3, Skull    x2</t>
-  </si>
-  <si>
     <t>04: 160(0A0): Egg(Lamia    x1)</t>
   </si>
   <si>
-    <t>05: 142(08E): GiantBat     x3, Cave Bat x3</t>
-  </si>
-  <si>
-    <t>06: 145(091): Ironback     x2, BlackLiz x2</t>
-  </si>
-  <si>
-    <t>07: 151(097): Staleman     x1, Skull    x2, Red Bone x2</t>
-  </si>
-  <si>
-    <t>08: 149(095): Staleman     x1</t>
-  </si>
-  <si>
     <t>GiantBat</t>
   </si>
   <si>
     <t>Ironback</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 1 -052</t>
+  </si>
+  <si>
+    <t>---------------------------------</t>
+  </si>
+  <si>
+    <t>01: 152(098): Mad Ogre     x2</t>
+  </si>
+  <si>
+    <t>02: 179(0B3): Sorcerer     x1, (Summon Mad Ogre x1), BladeMan x2</t>
+  </si>
+  <si>
+    <t>03: 160(0A0): Egg(Lamia    x1)</t>
+  </si>
+  <si>
+    <t>04: 166(0A6): Balloon      x3</t>
+  </si>
+  <si>
+    <t>05: 167(0A7): Balloon      x4</t>
+  </si>
+  <si>
+    <t>06: 155(09B): BlackCat     x2</t>
+  </si>
+  <si>
+    <t>07: 182(0B6): Sorcerer     x1, (Summon Green D. x1), BladeMan x2</t>
+  </si>
+  <si>
+    <t>08: 178(0B2): Egg(Green D. x1)</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 2 -053</t>
+  </si>
+  <si>
+    <t>01: 180(0B4): Sorcerer     x1, (Summon BlackCat x1), BladeMan x2</t>
+  </si>
+  <si>
+    <t>02: 167(0A7): Balloon      x4</t>
+  </si>
+  <si>
+    <t>03: 158(09E): Mad Ogre     x1,  BlackCat        x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04: 160(0A0): Egg(Lamia    x1)  </t>
+  </si>
+  <si>
+    <t>05: 168(0A8): Mad Ogre     x1,  BlackCat        x1,  Balloon  x2</t>
+  </si>
+  <si>
+    <t>06: 156(09C): BlackCat     x3</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 3-1 -054</t>
+  </si>
+  <si>
+    <t>-----------------------------------</t>
+  </si>
+  <si>
+    <t>01: 181(0B5): Sorcerer     x1, (Summon BladeMan x1), BladeMan x2</t>
+  </si>
+  <si>
+    <t>02: 159(09F): Mad Ogre     x2,  BlackCat        x2</t>
+  </si>
+  <si>
+    <t>03: 168(0A8): Mad Ogre     x1,  BlackCat        x1,  Balloon  x2</t>
+  </si>
+  <si>
+    <t>05: 153(099): Mad Ogre     x3</t>
+  </si>
+  <si>
+    <t>06: 169(0A9): Grudger      x1,  Mad Ogre        x1,  Balloon  x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 3-2 -055</t>
+  </si>
+  <si>
+    <t>01: 179(0B3): Sorcerer     x1, (Summon Mad Ogre x1), BladeMan x2</t>
+  </si>
+  <si>
+    <t>02: 164(0A4): BlackCat     x2,  Lamia           x1</t>
+  </si>
+  <si>
+    <t>03: 172(0AC): Balloon      x3,  Grudger         x1</t>
+  </si>
+  <si>
+    <t>05: 157(09D): Lamia        x1,  BlackCat        x1,  Mad Ogre x1</t>
+  </si>
+  <si>
+    <t>06: 166(0A6): Balloon      x3</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 4-1 -056</t>
+  </si>
+  <si>
+    <t>02: 172(0AC): Balloon      x3,  Grudger         x1</t>
+  </si>
+  <si>
+    <t>03: 165(0A5): BlackCat     x2,  Lamia           x2</t>
+  </si>
+  <si>
+    <t>05: 174(0AE): BladeMan     x3</t>
+  </si>
+  <si>
+    <t>06: 170(0AA): Grudger      x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 4-2 -057</t>
+  </si>
+  <si>
+    <t>01: 181(0B5): Sorceror     x1, (Summon BladeMan x1), BladeMan  x2</t>
+  </si>
+  <si>
+    <t>02: 175(0AF): BlackCat     x1,  BladeMan        x1,  Mad Ogre  x1</t>
+  </si>
+  <si>
+    <t>03: 163(0A3): Lamia        x1,  Mad Ogre        x1</t>
+  </si>
+  <si>
+    <t>05: 177(0B1): Mad Ogre     x1,  BladeMan        x1,  BlackCat  x1</t>
+  </si>
+  <si>
+    <t>06: 173(0AD): Grudger      x2,  Lamia           x1</t>
+  </si>
+  <si>
+    <t>07: 182(0B6): Sorcerer     x1, (Summon Green D. x1), BladeMan  x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 5 -058</t>
+  </si>
+  <si>
+    <t>03: 177(0B1): Mad Ogre     x1,  BladeMan        x1,  BlackCat x1</t>
+  </si>
+  <si>
+    <t>05: 171(0AB): Grudger      x3</t>
+  </si>
+  <si>
+    <t>06: 165(0A5): BlackCat     x2,  Lamia           x2</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 6 -059</t>
+  </si>
+  <si>
+    <t>01: 296(128): Egg(Lamia    x1), Q. Lamia         x1</t>
+  </si>
+  <si>
+    <t>02: 308(134): Sorcerer     x1, (Summon Q. Lamia  x1), BlackCat x2</t>
+  </si>
+  <si>
+    <t>03: 310(136): Grudger      x1,  BladeMan         x2</t>
+  </si>
+  <si>
+    <t>04: 297(129): Egg(Lamia    x3), Q. Lamia         x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05: 304(130): BladeMan     x1,  BlackCat         x1, Q. Lamia  x1 </t>
+  </si>
+  <si>
+    <t>06: 300(12C): Ironman      x1</t>
+  </si>
+  <si>
+    <t>07: 306(132): Sorcerer     x1, (Summon Q. Lamia  x1), BlackCat x2</t>
+  </si>
+  <si>
+    <t>08: 303(12F): Green D.     x1</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 7 -060</t>
+  </si>
+  <si>
+    <t>01: 307(133): Sorcerer x1, (Summon Ironman   x1), BlackCat x2</t>
+  </si>
+  <si>
+    <t>02: 309(135): Grudger  x2,  BladeMan         x2</t>
+  </si>
+  <si>
+    <t>03: 298(12A): Q. Lamia x1,  Egg(Lamia        x1), BlackCat x1</t>
+  </si>
+  <si>
+    <t>04: 299(12B): Q. Lamia x1,  Egg(Lamia        x1), Lamia    x2</t>
+  </si>
+  <si>
+    <t>05: 311(137): Grudger  x1,  BlackCat         x2,  BladeMan x1</t>
+  </si>
+  <si>
+    <t>06: 302(12E): Ironman  x1,  BladeMan         x2</t>
+  </si>
+  <si>
+    <t>07: 306(132): Sorcerer x1, (Summon Q. Lamia  x1), BlackCat x2</t>
+  </si>
+  <si>
+    <t>08: 303(12F): Green D. x1</t>
+  </si>
+  <si>
+    <t>Tower of Bab-il Revisited Floor 8 -061</t>
+  </si>
+  <si>
+    <t>01: 307(133): Sorcerer x1, (Summon Ironman  x1), BlackCat x2</t>
+  </si>
+  <si>
+    <t>02: 298(12A): Q. Lamia x1,  Egg(Lamia       x1), BlackCat x2</t>
+  </si>
+  <si>
+    <t>03: 311(137): Grudger  x1,  BlackCat        x2,  BladeMan x1</t>
+  </si>
+  <si>
+    <t>04: 309(135): Grudger  x2,  BladeMan        x2</t>
+  </si>
+  <si>
+    <t>05: 301(12D): Ironman  x2</t>
+  </si>
+  <si>
+    <t>06: 305(131): Ironman  x1,  Blackcat        x2</t>
+  </si>
+  <si>
+    <t>07: 306(132): Sorcerer x1, (Summon Q. Lamia x1), BlackCat x2</t>
   </si>
 </sst>
 </file>
@@ -645,7 +756,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -668,16 +779,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -701,26 +812,6 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -762,7 +853,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K42" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K42" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="I1:K42" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C525D014-8E05-4793-8C6B-F0E748D5A90D}" name="Name"/>
@@ -1070,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1180,7 @@
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1118,13 +1209,16 @@
         <v>40</v>
       </c>
       <c r="M1" t="s">
-        <v>149</v>
-      </c>
-      <c r="R1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="T1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1153,13 +1247,16 @@
         <v>1670</v>
       </c>
       <c r="M2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="T2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1188,13 +1285,16 @@
         <v>1260</v>
       </c>
       <c r="M3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="T3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1223,13 +1323,16 @@
         <v>3000</v>
       </c>
       <c r="M4" t="s">
-        <v>152</v>
-      </c>
-      <c r="R4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="T4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1258,13 +1361,16 @@
         <v>3000</v>
       </c>
       <c r="M5" t="s">
-        <v>153</v>
-      </c>
-      <c r="R5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="T5" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1293,13 +1399,16 @@
         <v>3000</v>
       </c>
       <c r="M6" t="s">
-        <v>154</v>
-      </c>
-      <c r="R6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="T6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1328,13 +1437,16 @@
         <v>9500</v>
       </c>
       <c r="M7" t="s">
-        <v>155</v>
-      </c>
-      <c r="R7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="T7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1363,13 +1475,16 @@
         <v>1000</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
-      </c>
-      <c r="R8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="T8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1398,13 +1513,16 @@
         <v>1000</v>
       </c>
       <c r="M9" t="s">
-        <v>157</v>
-      </c>
-      <c r="R9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="T9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1433,13 +1551,16 @@
         <v>18000</v>
       </c>
       <c r="M10" t="s">
-        <v>158</v>
-      </c>
-      <c r="R10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="T10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1468,7 +1589,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1500,10 +1621,16 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="T12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1526,7 +1653,7 @@
         <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="J13">
         <v>195</v>
@@ -1535,10 +1662,16 @@
         <v>1600</v>
       </c>
       <c r="M13" t="s">
+        <v>143</v>
+      </c>
+      <c r="T13" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="AA13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1558,7 +1691,7 @@
         <v>1200</v>
       </c>
       <c r="I14" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J14">
         <v>235</v>
@@ -1567,10 +1700,16 @@
         <v>1700</v>
       </c>
       <c r="M14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="T14" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1729,7 @@
         <v>680</v>
       </c>
       <c r="I15" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J15">
         <v>45</v>
@@ -1599,10 +1738,16 @@
         <v>1940</v>
       </c>
       <c r="M15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="T15" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1622,7 +1767,7 @@
         <v>4820</v>
       </c>
       <c r="I16" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="J16">
         <v>300</v>
@@ -1631,10 +1776,16 @@
         <v>1720</v>
       </c>
       <c r="M16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="T16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1654,7 +1805,7 @@
         <v>5500</v>
       </c>
       <c r="I17" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1663,10 +1814,16 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="T17" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1686,7 +1843,7 @@
         <v>1210</v>
       </c>
       <c r="I18" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="J18">
         <v>385</v>
@@ -1695,10 +1852,16 @@
         <v>1060</v>
       </c>
       <c r="M18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="T18" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1718,7 +1881,7 @@
         <v>1000</v>
       </c>
       <c r="I19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="J19">
         <v>270</v>
@@ -1727,10 +1890,16 @@
         <v>1420</v>
       </c>
       <c r="M19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="T19" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1750,7 +1919,7 @@
         <v>830</v>
       </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J20">
         <v>230</v>
@@ -1759,10 +1928,16 @@
         <v>2300</v>
       </c>
       <c r="M20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="T20" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1782,7 +1957,7 @@
         <v>960</v>
       </c>
       <c r="I21" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="J21">
         <v>380</v>
@@ -1791,10 +1966,16 @@
         <v>2100</v>
       </c>
       <c r="M21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="T21" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1814,7 +1995,7 @@
         <v>760</v>
       </c>
       <c r="I22" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="J22">
         <v>150</v>
@@ -1823,7 +2004,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1843,7 +2024,7 @@
         <v>1410</v>
       </c>
       <c r="I23" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="J23">
         <v>240</v>
@@ -1852,10 +2033,13 @@
         <v>2950</v>
       </c>
       <c r="M23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="T23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1875,7 +2059,7 @@
         <v>1010</v>
       </c>
       <c r="I24" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="J24">
         <v>225</v>
@@ -1884,10 +2068,13 @@
         <v>1250</v>
       </c>
       <c r="M24" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="T24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1907,7 +2094,7 @@
         <v>1510</v>
       </c>
       <c r="I25" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1916,10 +2103,13 @@
         <v>0</v>
       </c>
       <c r="M25" t="s">
+        <v>161</v>
+      </c>
+      <c r="T25" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1939,7 +2129,7 @@
         <v>1720</v>
       </c>
       <c r="I26" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1948,10 +2138,13 @@
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="T26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1971,7 +2164,7 @@
         <v>1300</v>
       </c>
       <c r="I27" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1980,10 +2173,13 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="T27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2003,7 +2199,7 @@
         <v>1100</v>
       </c>
       <c r="I28" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="J28">
         <v>4000</v>
@@ -2012,10 +2208,13 @@
         <v>3000</v>
       </c>
       <c r="M28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="T28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2035,7 +2234,7 @@
         <v>630</v>
       </c>
       <c r="I29" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="J29">
         <v>345</v>
@@ -2044,10 +2243,13 @@
         <v>2800</v>
       </c>
       <c r="M29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="T29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2067,7 +2269,7 @@
         <v>1100</v>
       </c>
       <c r="I30" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="J30">
         <v>1210</v>
@@ -2076,10 +2278,13 @@
         <v>2060</v>
       </c>
       <c r="M30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="T30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -2099,7 +2304,7 @@
         <v>750</v>
       </c>
       <c r="I31" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="J31">
         <v>270</v>
@@ -2108,10 +2313,13 @@
         <v>2370</v>
       </c>
       <c r="M31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="T31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2131,7 +2339,7 @@
         <v>820</v>
       </c>
       <c r="I32" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J32">
         <v>445</v>
@@ -2140,10 +2348,13 @@
         <v>2100</v>
       </c>
       <c r="M32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="T32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2163,7 +2374,7 @@
         <v>6000</v>
       </c>
       <c r="I33" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="J33">
         <v>120</v>
@@ -2172,7 +2383,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2192,7 +2403,7 @@
         <v>1570</v>
       </c>
       <c r="I34" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="J34">
         <v>365</v>
@@ -2200,8 +2411,14 @@
       <c r="K34">
         <v>1280</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>166</v>
+      </c>
+      <c r="T34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -2221,7 +2438,7 @@
         <v>1000</v>
       </c>
       <c r="I35" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="J35">
         <v>235</v>
@@ -2229,8 +2446,14 @@
       <c r="K35">
         <v>1100</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>160</v>
+      </c>
+      <c r="T35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2249,19 +2472,14 @@
       <c r="G36">
         <v>1350</v>
       </c>
-      <c r="M36">
-        <f>470+90</f>
-        <v>560</v>
-      </c>
-      <c r="N36">
-        <f>2600+2200</f>
-        <v>4800</v>
-      </c>
-      <c r="P36">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>167</v>
+      </c>
+      <c r="T36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2280,16 +2498,14 @@
       <c r="G37">
         <v>1500</v>
       </c>
-      <c r="N37">
-        <f>N36/4</f>
-        <v>1200</v>
-      </c>
-      <c r="P37">
-        <f>365*3+155*3</f>
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>168</v>
+      </c>
+      <c r="T37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2308,8 +2524,14 @@
       <c r="G38">
         <v>1500</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>169</v>
+      </c>
+      <c r="T38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -2328,8 +2550,14 @@
       <c r="G39">
         <v>1110</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>139</v>
+      </c>
+      <c r="T39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -2348,8 +2576,14 @@
       <c r="G40">
         <v>950</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>170</v>
+      </c>
+      <c r="T40" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -2368,8 +2602,14 @@
       <c r="G41">
         <v>760</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>171</v>
+      </c>
+      <c r="T41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -2387,6 +2627,20 @@
       </c>
       <c r="G42">
         <v>1100</v>
+      </c>
+      <c r="M42" t="s">
+        <v>150</v>
+      </c>
+      <c r="T42" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>151</v>
+      </c>
+      <c r="T43" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added color coding for unique strings; green for matches, red for non-matches, black for no text detected captured enemy data through second trip to bab-il, except for green dragon; captured a couple of 3-step peninsula monsters
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="231">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Ghast</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Milon Z.</t>
   </si>
   <si>
@@ -444,229 +441,283 @@
     <t>Skull</t>
   </si>
   <si>
-    <t>04: 160(0A0): Egg(Lamia    x1)</t>
-  </si>
-  <si>
     <t>GiantBat</t>
   </si>
   <si>
     <t>Ironback</t>
   </si>
   <si>
-    <t>Tower of Bab-il Revisited Floor 1 -052</t>
-  </si>
-  <si>
-    <t>---------------------------------</t>
-  </si>
-  <si>
-    <t>01: 152(098): Mad Ogre     x2</t>
-  </si>
-  <si>
-    <t>02: 179(0B3): Sorcerer     x1, (Summon Mad Ogre x1), BladeMan x2</t>
-  </si>
-  <si>
-    <t>03: 160(0A0): Egg(Lamia    x1)</t>
-  </si>
-  <si>
-    <t>04: 166(0A6): Balloon      x3</t>
-  </si>
-  <si>
-    <t>05: 167(0A7): Balloon      x4</t>
-  </si>
-  <si>
-    <t>06: 155(09B): BlackCat     x2</t>
-  </si>
-  <si>
-    <t>07: 182(0B6): Sorcerer     x1, (Summon Green D. x1), BladeMan x2</t>
-  </si>
-  <si>
-    <t>08: 178(0B2): Egg(Green D. x1)</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 2 -053</t>
-  </si>
-  <si>
-    <t>01: 180(0B4): Sorcerer     x1, (Summon BlackCat x1), BladeMan x2</t>
-  </si>
-  <si>
-    <t>02: 167(0A7): Balloon      x4</t>
-  </si>
-  <si>
-    <t>03: 158(09E): Mad Ogre     x1,  BlackCat        x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04: 160(0A0): Egg(Lamia    x1)  </t>
-  </si>
-  <si>
-    <t>05: 168(0A8): Mad Ogre     x1,  BlackCat        x1,  Balloon  x2</t>
-  </si>
-  <si>
-    <t>06: 156(09C): BlackCat     x3</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 3-1 -054</t>
-  </si>
-  <si>
-    <t>-----------------------------------</t>
-  </si>
-  <si>
-    <t>01: 181(0B5): Sorcerer     x1, (Summon BladeMan x1), BladeMan x2</t>
-  </si>
-  <si>
-    <t>02: 159(09F): Mad Ogre     x2,  BlackCat        x2</t>
-  </si>
-  <si>
-    <t>03: 168(0A8): Mad Ogre     x1,  BlackCat        x1,  Balloon  x2</t>
-  </si>
-  <si>
-    <t>05: 153(099): Mad Ogre     x3</t>
-  </si>
-  <si>
-    <t>06: 169(0A9): Grudger      x1,  Mad Ogre        x1,  Balloon  x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 3-2 -055</t>
-  </si>
-  <si>
-    <t>01: 179(0B3): Sorcerer     x1, (Summon Mad Ogre x1), BladeMan x2</t>
-  </si>
-  <si>
-    <t>02: 164(0A4): BlackCat     x2,  Lamia           x1</t>
-  </si>
-  <si>
-    <t>03: 172(0AC): Balloon      x3,  Grudger         x1</t>
-  </si>
-  <si>
-    <t>05: 157(09D): Lamia        x1,  BlackCat        x1,  Mad Ogre x1</t>
-  </si>
-  <si>
-    <t>06: 166(0A6): Balloon      x3</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 4-1 -056</t>
-  </si>
-  <si>
-    <t>02: 172(0AC): Balloon      x3,  Grudger         x1</t>
-  </si>
-  <si>
-    <t>03: 165(0A5): BlackCat     x2,  Lamia           x2</t>
-  </si>
-  <si>
-    <t>05: 174(0AE): BladeMan     x3</t>
-  </si>
-  <si>
-    <t>06: 170(0AA): Grudger      x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 4-2 -057</t>
-  </si>
-  <si>
-    <t>01: 181(0B5): Sorceror     x1, (Summon BladeMan x1), BladeMan  x2</t>
-  </si>
-  <si>
-    <t>02: 175(0AF): BlackCat     x1,  BladeMan        x1,  Mad Ogre  x1</t>
-  </si>
-  <si>
-    <t>03: 163(0A3): Lamia        x1,  Mad Ogre        x1</t>
-  </si>
-  <si>
-    <t>05: 177(0B1): Mad Ogre     x1,  BladeMan        x1,  BlackCat  x1</t>
-  </si>
-  <si>
-    <t>06: 173(0AD): Grudger      x2,  Lamia           x1</t>
-  </si>
-  <si>
-    <t>07: 182(0B6): Sorcerer     x1, (Summon Green D. x1), BladeMan  x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 5 -058</t>
-  </si>
-  <si>
-    <t>03: 177(0B1): Mad Ogre     x1,  BladeMan        x1,  BlackCat x1</t>
-  </si>
-  <si>
-    <t>05: 171(0AB): Grudger      x3</t>
-  </si>
-  <si>
-    <t>06: 165(0A5): BlackCat     x2,  Lamia           x2</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 6 -059</t>
-  </si>
-  <si>
-    <t>01: 296(128): Egg(Lamia    x1), Q. Lamia         x1</t>
-  </si>
-  <si>
-    <t>02: 308(134): Sorcerer     x1, (Summon Q. Lamia  x1), BlackCat x2</t>
-  </si>
-  <si>
-    <t>03: 310(136): Grudger      x1,  BladeMan         x2</t>
-  </si>
-  <si>
-    <t>04: 297(129): Egg(Lamia    x3), Q. Lamia         x1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05: 304(130): BladeMan     x1,  BlackCat         x1, Q. Lamia  x1 </t>
-  </si>
-  <si>
-    <t>06: 300(12C): Ironman      x1</t>
-  </si>
-  <si>
-    <t>07: 306(132): Sorcerer     x1, (Summon Q. Lamia  x1), BlackCat x2</t>
-  </si>
-  <si>
-    <t>08: 303(12F): Green D.     x1</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 7 -060</t>
-  </si>
-  <si>
-    <t>01: 307(133): Sorcerer x1, (Summon Ironman   x1), BlackCat x2</t>
-  </si>
-  <si>
-    <t>02: 309(135): Grudger  x2,  BladeMan         x2</t>
-  </si>
-  <si>
-    <t>03: 298(12A): Q. Lamia x1,  Egg(Lamia        x1), BlackCat x1</t>
-  </si>
-  <si>
-    <t>04: 299(12B): Q. Lamia x1,  Egg(Lamia        x1), Lamia    x2</t>
-  </si>
-  <si>
-    <t>05: 311(137): Grudger  x1,  BlackCat         x2,  BladeMan x1</t>
-  </si>
-  <si>
-    <t>06: 302(12E): Ironman  x1,  BladeMan         x2</t>
-  </si>
-  <si>
-    <t>07: 306(132): Sorcerer x1, (Summon Q. Lamia  x1), BlackCat x2</t>
-  </si>
-  <si>
-    <t>08: 303(12F): Green D. x1</t>
-  </si>
-  <si>
-    <t>Tower of Bab-il Revisited Floor 8 -061</t>
-  </si>
-  <si>
-    <t>01: 307(133): Sorcerer x1, (Summon Ironman  x1), BlackCat x2</t>
-  </si>
-  <si>
-    <t>02: 298(12A): Q. Lamia x1,  Egg(Lamia       x1), BlackCat x2</t>
-  </si>
-  <si>
-    <t>03: 311(137): Grudger  x1,  BlackCat        x2,  BladeMan x1</t>
-  </si>
-  <si>
-    <t>04: 309(135): Grudger  x2,  BladeMan        x2</t>
-  </si>
-  <si>
-    <t>05: 301(12D): Ironman  x2</t>
-  </si>
-  <si>
-    <t>06: 305(131): Ironman  x1,  Blackcat        x2</t>
-  </si>
-  <si>
-    <t>07: 306(132): Sorcerer x1, (Summon Q. Lamia x1), BlackCat x2</t>
+    <t>Balloon</t>
+  </si>
+  <si>
+    <t>BladeMan</t>
+  </si>
+  <si>
+    <t>Green D.</t>
+  </si>
+  <si>
+    <t>Sorcerer</t>
+  </si>
+  <si>
+    <t>Grudger</t>
+  </si>
+  <si>
+    <t>Q. Lamia</t>
+  </si>
+  <si>
+    <t>Ironman</t>
+  </si>
+  <si>
+    <t>need to avoid rydia, kain, while healing</t>
+  </si>
+  <si>
+    <t>Rubicant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-Step Peninsula -010 </t>
+  </si>
+  <si>
+    <t>----------------</t>
+  </si>
+  <si>
+    <t>01: 472(1D8): TrapRose     x1, GlomWing x2, Crawler  x2</t>
+  </si>
+  <si>
+    <t>02: 473(1D9): Medusa       x1, Gorgon   x1, Stoneman x1</t>
+  </si>
+  <si>
+    <t>07: 478(1DE): Egg(Green D. x1)</t>
+  </si>
+  <si>
+    <t>Underground2 -008</t>
+  </si>
+  <si>
+    <t>------------</t>
+  </si>
+  <si>
+    <t>01: 314(13A): TrapRose x2</t>
+  </si>
+  <si>
+    <t>02: 315(13B): RocLarva x4</t>
+  </si>
+  <si>
+    <t>03: 316(13C): RockMoth x2</t>
+  </si>
+  <si>
+    <t>04: 317(13D): RockMoth x2, RocLarva x2</t>
+  </si>
+  <si>
+    <t>05: 318(13E): TrapRose x1, RockMoth x2</t>
+  </si>
+  <si>
+    <t>06: 319(13F): TrapRose x1, RockMoth x2, RocLarva x2</t>
+  </si>
+  <si>
+    <t>07: 313(139): TrapRose x1, Centpede x2</t>
+  </si>
+  <si>
+    <t>08: 312(138): Centpede x1</t>
+  </si>
+  <si>
+    <t>Sylvan Cave -062</t>
+  </si>
+  <si>
+    <t>-----------</t>
+  </si>
+  <si>
+    <t>01: 320(140): ToadLady x1, TinyToad x3</t>
+  </si>
+  <si>
+    <t>02: 325(145): Ghost    x3</t>
+  </si>
+  <si>
+    <t>03: 328(148): Ghost    x3, DarkTree x2</t>
+  </si>
+  <si>
+    <t>04: 322(142): Molbol   x2</t>
+  </si>
+  <si>
+    <t>05: 326(146): Ghost    x4</t>
+  </si>
+  <si>
+    <t>06: 321(141): ToadLady x1, TinyToad x6</t>
+  </si>
+  <si>
+    <t>07: 330(14A): Centpede x1, Molbol   x2</t>
+  </si>
+  <si>
+    <t>08: 323(143): Molbol   x3</t>
+  </si>
+  <si>
+    <t>Sylvan Cave2 -063</t>
+  </si>
+  <si>
+    <t>01: 321(141): ToadLady x1, TinyToad x6</t>
+  </si>
+  <si>
+    <t>02: 331(14B): DarkTree x2, Molbol   x2</t>
+  </si>
+  <si>
+    <t>04: 329(149): DarkTree x2, Molbol   x1, Ghost    x1</t>
+  </si>
+  <si>
+    <t>05: 320(140): ToadLady x1, TinyToad x3</t>
+  </si>
+  <si>
+    <t>06: 327(147): Molbol   x1, Ghost    x1, DarkTree x1</t>
+  </si>
+  <si>
+    <t>07: 323(143): Molbol   x3</t>
+  </si>
+  <si>
+    <t>08: 324(144): Molbol   x1, Ghost    x2</t>
+  </si>
+  <si>
+    <t>Sealed Cave -064</t>
+  </si>
+  <si>
+    <t>01: 352(160): Were Bat x4</t>
+  </si>
+  <si>
+    <t>02: 354(162): VampLady x1, Were Bat x3</t>
+  </si>
+  <si>
+    <t>03: 358(166): Screamer x2</t>
+  </si>
+  <si>
+    <t>04: 353(161): Were Bat x3</t>
+  </si>
+  <si>
+    <t>05: 355(163): VampLady x1, Were Bat x6</t>
+  </si>
+  <si>
+    <t>06: 360(168): HugeNaga x2</t>
+  </si>
+  <si>
+    <t>07: 360(168): HugeNaga x2</t>
+  </si>
+  <si>
+    <t>08: 360(168): HugeNaga x2</t>
+  </si>
+  <si>
+    <t>Sealed Cave2 -065</t>
+  </si>
+  <si>
+    <t>01: 353(161): Were Bat x3</t>
+  </si>
+  <si>
+    <t>02: 355(163): VampLady x1, Were Bat x6</t>
+  </si>
+  <si>
+    <t>03: 359(167): Mantcore x1, Screamer x1</t>
+  </si>
+  <si>
+    <t>04: 360(168): HugeNaga x2</t>
+  </si>
+  <si>
+    <t>05: 356(164): VampLady x2, Were Bat x3</t>
+  </si>
+  <si>
+    <t>06: 361(169): Screamer x1, HugeNaga x1</t>
+  </si>
+  <si>
+    <t>07: 352(160): Were Bat x4</t>
+  </si>
+  <si>
+    <t>08: 354(162): VampLady x1, Were Bat x3</t>
+  </si>
+  <si>
+    <t>Sealed Cave3 -066</t>
+  </si>
+  <si>
+    <t>02: 356(164): VampLady x2, Were Bat x3</t>
+  </si>
+  <si>
+    <t>04: 362(16A): HugeNaga x1, Screamer x2</t>
+  </si>
+  <si>
+    <t>05: 354(162): VampLady x1, Were Bat x3</t>
+  </si>
+  <si>
+    <t>07: 356(164): VampLady x2, Were Bat x3</t>
+  </si>
+  <si>
+    <t>08: 361(169): Screamer x1, HugeNaga x1</t>
+  </si>
+  <si>
+    <t>Land of Monsters -067</t>
+  </si>
+  <si>
+    <t>01: 332(14C): Red Eye  x2</t>
+  </si>
+  <si>
+    <t>02: 344(158): Arachne  x1</t>
+  </si>
+  <si>
+    <t>03: 337(151): Warrior  x2,  Fiend           x2</t>
+  </si>
+  <si>
+    <t>04: 339(153): Conjurer x1, (Summon Imp      x1)</t>
+  </si>
+  <si>
+    <t>05: 340(154): Conjurer x1, (Summon RockMoth x1)</t>
+  </si>
+  <si>
+    <t>06: 342(156): Conjurer x1, (Summon HugeNaga x1)</t>
+  </si>
+  <si>
+    <t>07: 343(157): Conjurer x1, (Summon Clapper  x1)</t>
+  </si>
+  <si>
+    <t>08: 346(15A): Clapper  x1</t>
+  </si>
+  <si>
+    <t>Land of Monsters2 -068</t>
+  </si>
+  <si>
+    <t>-----------------</t>
+  </si>
+  <si>
+    <t>01: 335(14F): Hooligan x1</t>
+  </si>
+  <si>
+    <t>03: 337(154): Conjurer x1, (Summon RockMoth x1)</t>
+  </si>
+  <si>
+    <t>05: 341(155): Conjurer x1, (Summon Arachne  x1)</t>
+  </si>
+  <si>
+    <t>Land of Monsters3 -069</t>
+  </si>
+  <si>
+    <t>01: 333(14D): Red Eye  x3</t>
+  </si>
+  <si>
+    <t>02: 345(159): Arachne  x2</t>
+  </si>
+  <si>
+    <t>03: 338(152): Warrior  x2,  Fiend           x4</t>
+  </si>
+  <si>
+    <t>04: 336(150): Hooligan x2</t>
+  </si>
+  <si>
+    <t>08: 347(15B): Clapper  x2</t>
+  </si>
+  <si>
+    <t>Land of Monsters4 -070</t>
+  </si>
+  <si>
+    <t>01: 334(14E): Hooligan x1,  Red Eye         x1</t>
+  </si>
+  <si>
+    <t>HugeNaga</t>
+  </si>
+  <si>
+    <t>Talantla</t>
+  </si>
+  <si>
+    <t>Yellow D</t>
   </si>
 </sst>
 </file>
@@ -756,7 +807,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -779,16 +840,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -815,6 +876,26 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -829,8 +910,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C42" totalsRowShown="0">
-  <autoFilter ref="A1:C42" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7B0639-1979-4057-A03B-31BF23C3237A}" name="Table1" displayName="Table1" ref="A1:C83" totalsRowShown="0">
+  <autoFilter ref="A1:C83" xr:uid="{362A04B6-5B5F-4AB0-8471-78518A125A3F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{92B7C1DE-0885-429F-9F5C-CD5B673ABB7F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4EFBCB72-C5CC-4F4D-973E-B96095039970}" name="GP"/>
@@ -841,8 +922,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G42" totalsRowShown="0">
-  <autoFilter ref="E1:G42" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FEE72B92-1A72-4D03-A1D5-86708CB7EC7E}" name="Table2" displayName="Table2" ref="E1:G43" totalsRowShown="0">
+  <autoFilter ref="E1:G43" xr:uid="{6BD3315B-8F7C-4CD7-949E-414DBB07453F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7A239594-29E1-43D2-A7C7-BAD18B95F548}" name="Name"/>
     <tableColumn id="2" xr3:uid="{88D0DB9C-FE4B-4B88-80D2-A005BCE333DB}" name="GP"/>
@@ -853,8 +934,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K42" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="I1:K42" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K40" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
+  <autoFilter ref="I1:K40" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C525D014-8E05-4793-8C6B-F0E748D5A90D}" name="Name"/>
     <tableColumn id="2" xr3:uid="{3DE60367-455D-4CC0-8EA7-7199578C8493}" name="GP"/>
@@ -1161,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA43"/>
+  <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1261,7 @@
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1209,16 +1290,16 @@
         <v>40</v>
       </c>
       <c r="M1" t="s">
-        <v>142</v>
-      </c>
-      <c r="T1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="S1" t="s">
+        <v>182</v>
+      </c>
+      <c r="X1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1229,34 +1310,34 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="F2">
-        <v>170</v>
+        <v>330</v>
       </c>
       <c r="G2">
-        <v>320</v>
+        <v>1670</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="J2">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="K2">
-        <v>1670</v>
+        <v>3600</v>
       </c>
       <c r="M2" t="s">
-        <v>143</v>
-      </c>
-      <c r="T2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="S2" t="s">
+        <v>165</v>
+      </c>
+      <c r="X2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1267,34 +1348,34 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F3">
-        <v>365</v>
+        <v>200</v>
       </c>
       <c r="G3">
-        <v>2750</v>
+        <v>1260</v>
       </c>
       <c r="I3" t="s">
-        <v>108</v>
+        <v>229</v>
       </c>
       <c r="J3">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="K3">
-        <v>1260</v>
+        <v>2800</v>
       </c>
       <c r="M3" t="s">
-        <v>144</v>
-      </c>
-      <c r="T3" t="s">
-        <v>153</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="S3" t="s">
+        <v>183</v>
+      </c>
+      <c r="X3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1305,34 +1386,34 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="F4">
-        <v>180</v>
+        <v>3000</v>
       </c>
       <c r="G4">
-        <v>580</v>
+        <v>3000</v>
       </c>
       <c r="I4" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="J4">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="K4">
-        <v>3000</v>
+        <v>34000</v>
       </c>
       <c r="M4" t="s">
-        <v>145</v>
-      </c>
-      <c r="T4" t="s">
-        <v>173</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="S4" t="s">
+        <v>184</v>
+      </c>
+      <c r="X4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1343,34 +1424,22 @@
         <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="F5">
-        <v>190</v>
+        <v>3000</v>
       </c>
       <c r="G5">
-        <v>680</v>
-      </c>
-      <c r="I5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J5">
         <v>3000</v>
       </c>
-      <c r="K5">
-        <v>3000</v>
-      </c>
-      <c r="M5" t="s">
-        <v>146</v>
-      </c>
-      <c r="T5" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>185</v>
+      </c>
+      <c r="X5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1450,7 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="F6">
         <v>3000</v>
@@ -1389,26 +1458,17 @@
       <c r="G6">
         <v>3000</v>
       </c>
-      <c r="I6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J6">
-        <v>3000</v>
-      </c>
-      <c r="K6">
-        <v>3000</v>
-      </c>
       <c r="M6" t="s">
-        <v>147</v>
-      </c>
-      <c r="T6" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="S6" t="s">
+        <v>186</v>
+      </c>
+      <c r="X6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1419,34 +1479,25 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="F7">
-        <v>75</v>
+        <v>5500</v>
       </c>
       <c r="G7">
-        <v>800</v>
-      </c>
-      <c r="I7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J7">
-        <v>5500</v>
-      </c>
-      <c r="K7">
         <v>9500</v>
       </c>
       <c r="M7" t="s">
-        <v>148</v>
-      </c>
-      <c r="T7" t="s">
-        <v>175</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="S7" t="s">
+        <v>187</v>
+      </c>
+      <c r="X7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1457,34 +1508,25 @@
         <v>700</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="F8">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="G8">
-        <v>4000</v>
-      </c>
-      <c r="I8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J8">
-        <v>500</v>
-      </c>
-      <c r="K8">
         <v>1000</v>
       </c>
       <c r="M8" t="s">
-        <v>149</v>
-      </c>
-      <c r="T8" t="s">
-        <v>176</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="S8" t="s">
+        <v>188</v>
+      </c>
+      <c r="X8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1495,34 +1537,25 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="F9">
         <v>500</v>
       </c>
       <c r="G9">
-        <v>720</v>
-      </c>
-      <c r="I9" t="s">
-        <v>114</v>
-      </c>
-      <c r="J9">
-        <v>500</v>
-      </c>
-      <c r="K9">
         <v>1000</v>
       </c>
       <c r="M9" t="s">
-        <v>150</v>
-      </c>
-      <c r="T9" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="S9" t="s">
+        <v>189</v>
+      </c>
+      <c r="X9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1533,34 +1566,22 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="F10">
-        <v>145</v>
+        <v>6500</v>
       </c>
       <c r="G10">
-        <v>460</v>
-      </c>
-      <c r="I10" t="s">
-        <v>115</v>
-      </c>
-      <c r="J10">
-        <v>6500</v>
-      </c>
-      <c r="K10">
         <v>18000</v>
       </c>
       <c r="M10" t="s">
-        <v>151</v>
-      </c>
-      <c r="T10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="S10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1571,25 +1592,22 @@
         <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="F11">
-        <v>350</v>
+        <v>11000</v>
       </c>
       <c r="G11">
-        <v>1050</v>
-      </c>
-      <c r="I11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J11">
-        <v>11000</v>
-      </c>
-      <c r="K11">
         <v>20000</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>160</v>
+      </c>
+      <c r="X11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1600,37 +1618,25 @@
         <v>120</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="F12">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>870</v>
-      </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
       <c r="M12" t="s">
-        <v>152</v>
-      </c>
-      <c r="T12" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="S12" t="s">
+        <v>191</v>
+      </c>
+      <c r="X12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1641,37 +1647,25 @@
         <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="F13">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="G13">
-        <v>650</v>
-      </c>
-      <c r="H13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" t="s">
-        <v>118</v>
-      </c>
-      <c r="J13">
-        <v>195</v>
-      </c>
-      <c r="K13">
         <v>1600</v>
       </c>
       <c r="M13" t="s">
-        <v>143</v>
-      </c>
-      <c r="T13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="S13" t="s">
+        <v>155</v>
+      </c>
+      <c r="X13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1682,34 +1676,25 @@
         <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="F14">
-        <v>350</v>
+        <v>235</v>
       </c>
       <c r="G14">
-        <v>1200</v>
-      </c>
-      <c r="I14" t="s">
-        <v>119</v>
-      </c>
-      <c r="J14">
-        <v>235</v>
-      </c>
-      <c r="K14">
         <v>1700</v>
       </c>
       <c r="M14" t="s">
-        <v>153</v>
-      </c>
-      <c r="T14" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="S14" t="s">
+        <v>192</v>
+      </c>
+      <c r="X14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1720,34 +1705,22 @@
         <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="F15">
-        <v>230</v>
+        <v>45</v>
       </c>
       <c r="G15">
-        <v>680</v>
-      </c>
-      <c r="I15" t="s">
-        <v>120</v>
-      </c>
-      <c r="J15">
-        <v>45</v>
-      </c>
-      <c r="K15">
         <v>1940</v>
       </c>
-      <c r="M15" t="s">
-        <v>154</v>
-      </c>
-      <c r="T15" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>193</v>
+      </c>
+      <c r="X15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1758,34 +1731,25 @@
         <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="F16">
-        <v>3000</v>
+        <v>300</v>
       </c>
       <c r="G16">
-        <v>4820</v>
-      </c>
-      <c r="I16" t="s">
-        <v>121</v>
-      </c>
-      <c r="J16">
-        <v>300</v>
-      </c>
-      <c r="K16">
         <v>1720</v>
       </c>
       <c r="M16" t="s">
-        <v>155</v>
-      </c>
-      <c r="T16" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="S16" t="s">
+        <v>194</v>
+      </c>
+      <c r="X16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1796,34 +1760,25 @@
         <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="F17">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>5500</v>
-      </c>
-      <c r="I17" t="s">
-        <v>122</v>
-      </c>
-      <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
       <c r="M17" t="s">
-        <v>156</v>
-      </c>
-      <c r="T17" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="S17" t="s">
+        <v>195</v>
+      </c>
+      <c r="X17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1834,34 +1789,25 @@
         <v>1200</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="F18">
-        <v>220</v>
+        <v>385</v>
       </c>
       <c r="G18">
-        <v>1210</v>
-      </c>
-      <c r="I18" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18">
-        <v>385</v>
-      </c>
-      <c r="K18">
         <v>1060</v>
       </c>
       <c r="M18" t="s">
-        <v>157</v>
-      </c>
-      <c r="T18" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="S18" t="s">
+        <v>196</v>
+      </c>
+      <c r="X18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1872,34 +1818,25 @@
         <v>260</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="F19">
-        <v>150</v>
+        <v>270</v>
       </c>
       <c r="G19">
-        <v>1000</v>
-      </c>
-      <c r="I19" t="s">
-        <v>124</v>
-      </c>
-      <c r="J19">
-        <v>270</v>
-      </c>
-      <c r="K19">
         <v>1420</v>
       </c>
       <c r="M19" t="s">
-        <v>158</v>
-      </c>
-      <c r="T19" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="S19" t="s">
+        <v>197</v>
+      </c>
+      <c r="X19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1910,34 +1847,25 @@
         <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="F20">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="G20">
-        <v>830</v>
-      </c>
-      <c r="I20" t="s">
-        <v>125</v>
-      </c>
-      <c r="J20">
-        <v>230</v>
-      </c>
-      <c r="K20">
         <v>2300</v>
       </c>
       <c r="M20" t="s">
-        <v>150</v>
-      </c>
-      <c r="T20" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="S20" t="s">
+        <v>198</v>
+      </c>
+      <c r="X20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1948,34 +1876,22 @@
         <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="F21">
-        <v>220</v>
+        <v>380</v>
       </c>
       <c r="G21">
-        <v>960</v>
-      </c>
-      <c r="I21" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21">
-        <v>380</v>
-      </c>
-      <c r="K21">
         <v>2100</v>
       </c>
       <c r="M21" t="s">
-        <v>151</v>
-      </c>
-      <c r="T21" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="S21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1986,25 +1902,22 @@
         <v>400</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="F22">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="G22">
-        <v>760</v>
-      </c>
-      <c r="I22" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22">
-        <v>150</v>
-      </c>
-      <c r="K22">
         <v>1120</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>171</v>
+      </c>
+      <c r="X22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2015,31 +1928,25 @@
         <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="F23">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="G23">
-        <v>1410</v>
-      </c>
-      <c r="I23" t="s">
-        <v>128</v>
-      </c>
-      <c r="J23">
-        <v>240</v>
-      </c>
-      <c r="K23">
         <v>2950</v>
       </c>
       <c r="M23" t="s">
-        <v>159</v>
-      </c>
-      <c r="T23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="S23" t="s">
+        <v>200</v>
+      </c>
+      <c r="X23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2050,31 +1957,25 @@
         <v>240</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="F24">
-        <v>85</v>
+        <v>225</v>
       </c>
       <c r="G24">
-        <v>1010</v>
-      </c>
-      <c r="I24" t="s">
-        <v>129</v>
-      </c>
-      <c r="J24">
-        <v>225</v>
-      </c>
-      <c r="K24">
         <v>1250</v>
       </c>
       <c r="M24" t="s">
-        <v>160</v>
-      </c>
-      <c r="T24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="S24" t="s">
+        <v>155</v>
+      </c>
+      <c r="X24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2085,31 +1986,22 @@
         <v>190</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="F25">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>1510</v>
-      </c>
-      <c r="I25" t="s">
-        <v>130</v>
-      </c>
-      <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="M25" t="s">
-        <v>161</v>
-      </c>
-      <c r="T25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S25" t="s">
+        <v>183</v>
+      </c>
+      <c r="X25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2120,31 +2012,25 @@
         <v>120</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="F26">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>1720</v>
-      </c>
-      <c r="I26" t="s">
-        <v>131</v>
-      </c>
-      <c r="J26">
         <v>0</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
       <c r="M26" t="s">
-        <v>162</v>
-      </c>
-      <c r="T26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="S26" t="s">
+        <v>201</v>
+      </c>
+      <c r="X26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2155,31 +2041,25 @@
         <v>240</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="F27">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>1300</v>
-      </c>
-      <c r="I27" t="s">
-        <v>133</v>
-      </c>
-      <c r="J27">
         <v>0</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
       <c r="M27" t="s">
-        <v>163</v>
-      </c>
-      <c r="T27" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="S27" t="s">
+        <v>194</v>
+      </c>
+      <c r="X27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2190,31 +2070,25 @@
         <v>160</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="F28">
-        <v>240</v>
+        <v>4000</v>
       </c>
       <c r="G28">
-        <v>1100</v>
-      </c>
-      <c r="I28" t="s">
-        <v>132</v>
-      </c>
-      <c r="J28">
-        <v>4000</v>
-      </c>
-      <c r="K28">
         <v>3000</v>
       </c>
       <c r="M28" t="s">
-        <v>139</v>
-      </c>
-      <c r="T28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="S28" t="s">
+        <v>202</v>
+      </c>
+      <c r="X28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2225,31 +2099,25 @@
         <v>150</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="F29">
-        <v>155</v>
+        <v>345</v>
       </c>
       <c r="G29">
-        <v>630</v>
-      </c>
-      <c r="I29" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29">
-        <v>345</v>
-      </c>
-      <c r="K29">
         <v>2800</v>
       </c>
       <c r="M29" t="s">
-        <v>164</v>
-      </c>
-      <c r="T29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="S29" t="s">
+        <v>203</v>
+      </c>
+      <c r="X29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2260,31 +2128,25 @@
         <v>1500</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="F30">
-        <v>235</v>
+        <v>1210</v>
       </c>
       <c r="G30">
-        <v>1100</v>
-      </c>
-      <c r="I30" t="s">
-        <v>135</v>
-      </c>
-      <c r="J30">
-        <v>1210</v>
-      </c>
-      <c r="K30">
         <v>2060</v>
       </c>
       <c r="M30" t="s">
-        <v>165</v>
-      </c>
-      <c r="T30" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="S30" t="s">
+        <v>197</v>
+      </c>
+      <c r="X30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -2295,31 +2157,25 @@
         <v>240</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="F31">
-        <v>205</v>
+        <v>270</v>
       </c>
       <c r="G31">
-        <v>750</v>
-      </c>
-      <c r="I31" t="s">
-        <v>136</v>
-      </c>
-      <c r="J31">
-        <v>270</v>
-      </c>
-      <c r="K31">
         <v>2370</v>
       </c>
       <c r="M31" t="s">
-        <v>150</v>
-      </c>
-      <c r="T31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="S31" t="s">
+        <v>204</v>
+      </c>
+      <c r="X31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2330,31 +2186,22 @@
         <v>290</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="F32">
-        <v>195</v>
+        <v>445</v>
       </c>
       <c r="G32">
-        <v>820</v>
-      </c>
-      <c r="I32" t="s">
-        <v>137</v>
-      </c>
-      <c r="J32">
-        <v>445</v>
-      </c>
-      <c r="K32">
         <v>2100</v>
       </c>
       <c r="M32" t="s">
-        <v>151</v>
-      </c>
-      <c r="T32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="S32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2365,25 +2212,19 @@
         <v>320</v>
       </c>
       <c r="E33" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="F33">
-        <v>5000</v>
+        <v>120</v>
       </c>
       <c r="G33">
-        <v>6000</v>
-      </c>
-      <c r="I33" t="s">
-        <v>138</v>
-      </c>
-      <c r="J33">
-        <v>120</v>
-      </c>
-      <c r="K33">
         <v>1580</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2394,31 +2235,22 @@
         <v>280</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="F34">
-        <v>280</v>
+        <v>365</v>
       </c>
       <c r="G34">
-        <v>1570</v>
-      </c>
-      <c r="I34" t="s">
-        <v>140</v>
-      </c>
-      <c r="J34">
-        <v>365</v>
-      </c>
-      <c r="K34">
         <v>1280</v>
       </c>
       <c r="M34" t="s">
-        <v>166</v>
-      </c>
-      <c r="T34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="S34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -2429,31 +2261,19 @@
         <v>370</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="F35">
-        <v>175</v>
+        <v>235</v>
       </c>
       <c r="G35">
-        <v>1000</v>
-      </c>
-      <c r="I35" t="s">
-        <v>141</v>
-      </c>
-      <c r="J35">
-        <v>235</v>
-      </c>
-      <c r="K35">
         <v>1100</v>
       </c>
-      <c r="M35" t="s">
-        <v>160</v>
-      </c>
-      <c r="T35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2464,22 +2284,19 @@
         <v>450</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F36">
-        <v>230</v>
+        <v>315</v>
       </c>
       <c r="G36">
-        <v>1350</v>
-      </c>
-      <c r="M36" t="s">
-        <v>167</v>
-      </c>
-      <c r="T36" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <v>2480</v>
+      </c>
+      <c r="S36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2490,24 +2307,21 @@
         <v>370</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="F37">
-        <v>290</v>
+        <v>215</v>
       </c>
       <c r="G37">
-        <v>1500</v>
-      </c>
-      <c r="M37" t="s">
-        <v>168</v>
-      </c>
-      <c r="T37" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>2600</v>
+      </c>
+      <c r="S37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2516,22 +2330,16 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
-      </c>
-      <c r="F38">
-        <v>275</v>
-      </c>
-      <c r="G38">
-        <v>1500</v>
-      </c>
-      <c r="M38" t="s">
-        <v>169</v>
-      </c>
-      <c r="T38" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="S38" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -2542,22 +2350,19 @@
         <v>410</v>
       </c>
       <c r="E39" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="F39">
-        <v>195</v>
+        <v>275</v>
       </c>
       <c r="G39">
-        <v>1110</v>
-      </c>
-      <c r="M39" t="s">
-        <v>139</v>
-      </c>
-      <c r="T39" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <v>2370</v>
+      </c>
+      <c r="S39" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -2568,22 +2373,19 @@
         <v>610</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="F40">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="G40">
-        <v>950</v>
-      </c>
-      <c r="M40" t="s">
-        <v>170</v>
-      </c>
-      <c r="T40" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>2460</v>
+      </c>
+      <c r="S40" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -2594,22 +2396,19 @@
         <v>740</v>
       </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="F41">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="G41">
-        <v>760</v>
-      </c>
-      <c r="M41" t="s">
-        <v>171</v>
-      </c>
-      <c r="T41" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>2900</v>
+      </c>
+      <c r="S41" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -2620,35 +2419,484 @@
         <v>510</v>
       </c>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="F42">
+        <v>385</v>
+      </c>
+      <c r="G42">
+        <v>3700</v>
+      </c>
+      <c r="S42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43">
+        <v>170</v>
+      </c>
+      <c r="C43">
+        <v>320</v>
+      </c>
+      <c r="E43" t="s">
+        <v>148</v>
+      </c>
+      <c r="F43">
+        <v>7000</v>
+      </c>
+      <c r="G43">
+        <v>25000</v>
+      </c>
+      <c r="S43" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44">
+        <v>365</v>
+      </c>
+      <c r="C44">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45">
+        <v>180</v>
+      </c>
+      <c r="C45">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46">
+        <v>190</v>
+      </c>
+      <c r="C46">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47">
+        <v>3000</v>
+      </c>
+      <c r="C47">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48">
+        <v>75</v>
+      </c>
+      <c r="C48">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49">
+        <v>3000</v>
+      </c>
+      <c r="C49">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50">
+        <v>500</v>
+      </c>
+      <c r="C50">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51">
+        <v>145</v>
+      </c>
+      <c r="C51">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52">
+        <v>350</v>
+      </c>
+      <c r="C52">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53">
+        <v>300</v>
+      </c>
+      <c r="C53">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54">
+        <v>230</v>
+      </c>
+      <c r="C54">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55">
+        <v>350</v>
+      </c>
+      <c r="C55">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56">
+        <v>230</v>
+      </c>
+      <c r="C56">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57">
+        <v>3000</v>
+      </c>
+      <c r="C57">
+        <v>4820</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58">
+        <v>4000</v>
+      </c>
+      <c r="C58">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59">
+        <v>220</v>
+      </c>
+      <c r="C59">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60">
+        <v>150</v>
+      </c>
+      <c r="C60">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61">
+        <v>255</v>
+      </c>
+      <c r="C61">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62">
+        <v>220</v>
+      </c>
+      <c r="C62">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63">
+        <v>225</v>
+      </c>
+      <c r="C63">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64">
+        <v>150</v>
+      </c>
+      <c r="C64">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65">
+        <v>85</v>
+      </c>
+      <c r="C65">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66">
+        <v>255</v>
+      </c>
+      <c r="C66">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67">
+        <v>245</v>
+      </c>
+      <c r="C67">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68">
+        <v>45</v>
+      </c>
+      <c r="C68">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69">
+        <v>240</v>
+      </c>
+      <c r="C69">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70">
+        <v>155</v>
+      </c>
+      <c r="C70">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71">
+        <v>235</v>
+      </c>
+      <c r="C71">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72">
+        <v>205</v>
+      </c>
+      <c r="C72">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73">
+        <v>195</v>
+      </c>
+      <c r="C73">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74">
+        <v>5000</v>
+      </c>
+      <c r="C74">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75">
+        <v>280</v>
+      </c>
+      <c r="C75">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76">
         <v>175</v>
       </c>
-      <c r="G42">
+      <c r="C76">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77">
+        <v>230</v>
+      </c>
+      <c r="C77">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78">
+        <v>290</v>
+      </c>
+      <c r="C78">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79">
+        <v>275</v>
+      </c>
+      <c r="C79">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>102</v>
+      </c>
+      <c r="B80">
+        <v>195</v>
+      </c>
+      <c r="C80">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81">
+        <v>180</v>
+      </c>
+      <c r="C81">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82">
+        <v>50</v>
+      </c>
+      <c r="C82">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>105</v>
+      </c>
+      <c r="B83">
+        <v>175</v>
+      </c>
+      <c r="C83">
         <v>1100</v>
       </c>
-      <c r="M42" t="s">
-        <v>150</v>
-      </c>
-      <c r="T42" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="M43" t="s">
-        <v>151</v>
-      </c>
-      <c r="T43" t="s">
-        <v>196</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A37:A38">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A42 E2:E42 I2:I42">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+  <conditionalFormatting sqref="I2:I40 E2:E43 A2:A83">
+    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">

</xml_diff>

<commit_message>
more underworld data; need to figure out how to confirm glomwing, crawler
</commit_message>
<xml_diff>
--- a/ff_ocr/manual_data.xlsx
+++ b/ff_ocr/manual_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="233">
   <si>
     <t>FloatEye x 2</t>
   </si>
@@ -480,45 +480,12 @@
     <t>----------------</t>
   </si>
   <si>
-    <t>01: 472(1D8): TrapRose     x1, GlomWing x2, Crawler  x2</t>
-  </si>
-  <si>
     <t>02: 473(1D9): Medusa       x1, Gorgon   x1, Stoneman x1</t>
   </si>
   <si>
-    <t>07: 478(1DE): Egg(Green D. x1)</t>
-  </si>
-  <si>
-    <t>Underground2 -008</t>
-  </si>
-  <si>
     <t>------------</t>
   </si>
   <si>
-    <t>01: 314(13A): TrapRose x2</t>
-  </si>
-  <si>
-    <t>02: 315(13B): RocLarva x4</t>
-  </si>
-  <si>
-    <t>03: 316(13C): RockMoth x2</t>
-  </si>
-  <si>
-    <t>04: 317(13D): RockMoth x2, RocLarva x2</t>
-  </si>
-  <si>
-    <t>05: 318(13E): TrapRose x1, RockMoth x2</t>
-  </si>
-  <si>
-    <t>06: 319(13F): TrapRose x1, RockMoth x2, RocLarva x2</t>
-  </si>
-  <si>
-    <t>07: 313(139): TrapRose x1, Centpede x2</t>
-  </si>
-  <si>
-    <t>08: 312(138): Centpede x1</t>
-  </si>
-  <si>
     <t>Sylvan Cave -062</t>
   </si>
   <si>
@@ -718,6 +685,45 @@
   </si>
   <si>
     <t>Yellow D</t>
+  </si>
+  <si>
+    <t>TrapRose</t>
+  </si>
+  <si>
+    <t>GlomWing</t>
+  </si>
+  <si>
+    <t>Crawler</t>
+  </si>
+  <si>
+    <t>Gorgon</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>GlomWing * 2</t>
+  </si>
+  <si>
+    <t>Crawler * 2</t>
+  </si>
+  <si>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>RocLarva</t>
+  </si>
+  <si>
+    <t>RockMoth</t>
+  </si>
+  <si>
+    <t>Centpede</t>
+  </si>
+  <si>
+    <t>G+C</t>
   </si>
 </sst>
 </file>
@@ -755,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -794,20 +800,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -876,26 +932,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -934,7 +970,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K40" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CDCC935-517B-4EED-973C-F1D255DC62EC}" name="Table3" displayName="Table3" ref="I1:K40" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
   <autoFilter ref="I1:K40" xr:uid="{10FA31CB-90BB-495E-92A7-205AC0FB2F18}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C525D014-8E05-4793-8C6B-F0E748D5A90D}" name="Name"/>
@@ -1245,7 +1281,7 @@
   <dimension ref="A1:AC83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1297,7 @@
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1293,13 +1329,13 @@
         <v>149</v>
       </c>
       <c r="S1" t="s">
-        <v>182</v>
-      </c>
-      <c r="X1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1319,7 +1355,7 @@
         <v>1670</v>
       </c>
       <c r="I2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="J2">
         <v>240</v>
@@ -1331,13 +1367,13 @@
         <v>151</v>
       </c>
       <c r="S2" t="s">
-        <v>165</v>
-      </c>
-      <c r="X2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1357,7 +1393,7 @@
         <v>1260</v>
       </c>
       <c r="I3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="J3">
         <v>600</v>
@@ -1365,17 +1401,14 @@
       <c r="K3">
         <v>2800</v>
       </c>
-      <c r="M3" t="s">
-        <v>152</v>
-      </c>
       <c r="S3" t="s">
-        <v>183</v>
-      </c>
-      <c r="X3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1395,7 +1428,7 @@
         <v>3000</v>
       </c>
       <c r="I4" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="J4">
         <v>1500</v>
@@ -1407,13 +1440,13 @@
         <v>153</v>
       </c>
       <c r="S4" t="s">
-        <v>184</v>
-      </c>
-      <c r="X4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1432,14 +1465,26 @@
       <c r="G5">
         <v>3000</v>
       </c>
+      <c r="I5" t="s">
+        <v>220</v>
+      </c>
+      <c r="J5">
+        <v>35</v>
+      </c>
+      <c r="K5">
+        <v>1210</v>
+      </c>
+      <c r="M5" t="s">
+        <v>155</v>
+      </c>
       <c r="S5" t="s">
-        <v>185</v>
-      </c>
-      <c r="X5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1458,17 +1503,29 @@
       <c r="G6">
         <v>3000</v>
       </c>
+      <c r="I6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J6">
+        <v>510</v>
+      </c>
+      <c r="K6">
+        <v>2850</v>
+      </c>
+      <c r="L6" t="s">
+        <v>224</v>
+      </c>
       <c r="M6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="S6" t="s">
-        <v>186</v>
-      </c>
-      <c r="X6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1487,17 +1544,29 @@
       <c r="G7">
         <v>9500</v>
       </c>
+      <c r="I7" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7">
+        <v>540</v>
+      </c>
+      <c r="K7">
+        <v>3450</v>
+      </c>
+      <c r="L7" t="s">
+        <v>224</v>
+      </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="S7" t="s">
-        <v>187</v>
-      </c>
-      <c r="X7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1516,17 +1585,26 @@
       <c r="G8">
         <v>1000</v>
       </c>
+      <c r="I8" t="s">
+        <v>223</v>
+      </c>
+      <c r="J8">
+        <v>250</v>
+      </c>
+      <c r="K8">
+        <v>3050</v>
+      </c>
       <c r="M8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="S8" t="s">
-        <v>188</v>
-      </c>
-      <c r="X8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1545,17 +1623,26 @@
       <c r="G9">
         <v>1000</v>
       </c>
+      <c r="I9" t="s">
+        <v>229</v>
+      </c>
+      <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>2830</v>
+      </c>
       <c r="M9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="S9" t="s">
-        <v>189</v>
-      </c>
-      <c r="X9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1574,14 +1661,23 @@
       <c r="G10">
         <v>18000</v>
       </c>
+      <c r="I10" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10">
+        <v>315</v>
+      </c>
+      <c r="K10">
+        <v>3200</v>
+      </c>
       <c r="M10" t="s">
-        <v>159</v>
-      </c>
-      <c r="S10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1600,14 +1696,23 @@
       <c r="G11">
         <v>20000</v>
       </c>
+      <c r="I11" t="s">
+        <v>231</v>
+      </c>
+      <c r="J11">
+        <v>345</v>
+      </c>
+      <c r="K11">
+        <v>2800</v>
+      </c>
       <c r="M11" t="s">
-        <v>160</v>
-      </c>
-      <c r="X11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="S11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1627,16 +1732,16 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="S12" t="s">
-        <v>191</v>
-      </c>
-      <c r="X12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1655,17 +1760,14 @@
       <c r="G13">
         <v>1600</v>
       </c>
-      <c r="M13" t="s">
-        <v>162</v>
-      </c>
       <c r="S13" t="s">
-        <v>155</v>
-      </c>
-      <c r="X13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1688,13 +1790,13 @@
         <v>163</v>
       </c>
       <c r="S14" t="s">
-        <v>192</v>
-      </c>
-      <c r="X14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1713,14 +1815,17 @@
       <c r="G15">
         <v>1940</v>
       </c>
+      <c r="M15" t="s">
+        <v>164</v>
+      </c>
       <c r="S15" t="s">
-        <v>193</v>
-      </c>
-      <c r="X15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1740,16 +1845,16 @@
         <v>1720</v>
       </c>
       <c r="M16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S16" t="s">
-        <v>194</v>
-      </c>
-      <c r="X16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1769,16 +1874,16 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="S17" t="s">
-        <v>195</v>
-      </c>
-      <c r="X17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1798,16 +1903,16 @@
         <v>1060</v>
       </c>
       <c r="M18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S18" t="s">
-        <v>196</v>
-      </c>
-      <c r="X18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1827,16 +1932,16 @@
         <v>1420</v>
       </c>
       <c r="M19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="S19" t="s">
-        <v>197</v>
-      </c>
-      <c r="X19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1856,16 +1961,16 @@
         <v>2300</v>
       </c>
       <c r="M20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S20" t="s">
-        <v>198</v>
-      </c>
-      <c r="X20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1885,13 +1990,13 @@
         <v>2100</v>
       </c>
       <c r="M21" t="s">
-        <v>170</v>
-      </c>
-      <c r="S21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1911,13 +2016,13 @@
         <v>1120</v>
       </c>
       <c r="M22" t="s">
-        <v>171</v>
-      </c>
-      <c r="X22" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="S22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1936,17 +2041,14 @@
       <c r="G23">
         <v>2950</v>
       </c>
-      <c r="M23" t="s">
-        <v>172</v>
-      </c>
       <c r="S23" t="s">
-        <v>200</v>
-      </c>
-      <c r="X23" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1966,16 +2068,16 @@
         <v>1250</v>
       </c>
       <c r="M24" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="S24" t="s">
-        <v>155</v>
-      </c>
-      <c r="X24" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1994,14 +2096,17 @@
       <c r="G25">
         <v>0</v>
       </c>
+      <c r="M25" t="s">
+        <v>150</v>
+      </c>
       <c r="S25" t="s">
-        <v>183</v>
-      </c>
-      <c r="X25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2021,16 +2126,16 @@
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="S26" t="s">
-        <v>201</v>
-      </c>
-      <c r="X26" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2050,16 +2155,16 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="S27" t="s">
-        <v>194</v>
-      </c>
-      <c r="X27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2079,16 +2184,16 @@
         <v>3000</v>
       </c>
       <c r="M28" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="S28" t="s">
-        <v>202</v>
-      </c>
-      <c r="X28" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2108,16 +2213,16 @@
         <v>2800</v>
       </c>
       <c r="M29" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="S29" t="s">
-        <v>203</v>
-      </c>
-      <c r="X29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2137,16 +2242,16 @@
         <v>2060</v>
       </c>
       <c r="M30" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="S30" t="s">
-        <v>197</v>
-      </c>
-      <c r="X30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -2166,16 +2271,16 @@
         <v>2370</v>
       </c>
       <c r="M31" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="S31" t="s">
-        <v>204</v>
-      </c>
-      <c r="X31" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2195,10 +2300,10 @@
         <v>2100</v>
       </c>
       <c r="M32" t="s">
-        <v>179</v>
-      </c>
-      <c r="S32" t="s">
-        <v>205</v>
+        <v>202</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
@@ -2221,7 +2326,7 @@
         <v>1580</v>
       </c>
       <c r="M33" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
@@ -2243,12 +2348,6 @@
       <c r="G34">
         <v>1280</v>
       </c>
-      <c r="M34" t="s">
-        <v>181</v>
-      </c>
-      <c r="S34" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2269,9 +2368,6 @@
       <c r="G35">
         <v>1100</v>
       </c>
-      <c r="S35" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2292,9 +2388,6 @@
       <c r="G36">
         <v>2480</v>
       </c>
-      <c r="S36" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2315,8 +2408,11 @@
       <c r="G37">
         <v>2600</v>
       </c>
-      <c r="S37" t="s">
-        <v>208</v>
+      <c r="O37" t="s">
+        <v>227</v>
+      </c>
+      <c r="P37" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -2332,8 +2428,22 @@
       <c r="E38" t="s">
         <v>142</v>
       </c>
-      <c r="S38" t="s">
-        <v>209</v>
+      <c r="F38">
+        <v>370</v>
+      </c>
+      <c r="G38">
+        <v>4800</v>
+      </c>
+      <c r="M38" t="s">
+        <v>220</v>
+      </c>
+      <c r="O38">
+        <f>J5</f>
+        <v>35</v>
+      </c>
+      <c r="P38">
+        <f>K5</f>
+        <v>1210</v>
       </c>
       <c r="AC38" t="s">
         <v>147</v>
@@ -2358,8 +2468,15 @@
       <c r="G39">
         <v>2370</v>
       </c>
-      <c r="S39" t="s">
-        <v>210</v>
+      <c r="M39" t="s">
+        <v>225</v>
+      </c>
+      <c r="O39">
+        <f>J6*2</f>
+        <v>1020</v>
+      </c>
+      <c r="P39">
+        <v>6300</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
@@ -2381,8 +2498,16 @@
       <c r="G40">
         <v>2460</v>
       </c>
-      <c r="S40" t="s">
-        <v>211</v>
+      <c r="M40" t="s">
+        <v>226</v>
+      </c>
+      <c r="O40">
+        <f>J7*2</f>
+        <v>1080</v>
+      </c>
+      <c r="P40">
+        <f>K7*2</f>
+        <v>6900</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
@@ -2404,8 +2529,13 @@
       <c r="G41">
         <v>2900</v>
       </c>
-      <c r="S41" t="s">
-        <v>212</v>
+      <c r="O41">
+        <f>O40+O39+O38</f>
+        <v>2135</v>
+      </c>
+      <c r="P41">
+        <f>P40+P39+P38</f>
+        <v>14410</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
@@ -2427,8 +2557,11 @@
       <c r="G42">
         <v>3700</v>
       </c>
-      <c r="S42" t="s">
-        <v>213</v>
+      <c r="O42">
+        <v>2135</v>
+      </c>
+      <c r="P42">
+        <v>2946</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
@@ -2450,8 +2583,9 @@
       <c r="G43">
         <v>25000</v>
       </c>
-      <c r="S43" t="s">
-        <v>214</v>
+      <c r="P43">
+        <f>P42*5</f>
+        <v>14730</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
@@ -2464,6 +2598,13 @@
       <c r="C44">
         <v>2750</v>
       </c>
+      <c r="O44" t="s">
+        <v>232</v>
+      </c>
+      <c r="P44">
+        <f>P43-P38</f>
+        <v>13520</v>
+      </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2475,6 +2616,10 @@
       <c r="C45">
         <v>580</v>
       </c>
+      <c r="P45">
+        <f>P44/2</f>
+        <v>6760</v>
+      </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -2486,6 +2631,10 @@
       <c r="C46">
         <v>680</v>
       </c>
+      <c r="P46">
+        <f>P45/2</f>
+        <v>3380</v>
+      </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2497,6 +2646,10 @@
       <c r="C47">
         <v>3000</v>
       </c>
+      <c r="P47">
+        <f>1020/1080</f>
+        <v>0.94444444444444442</v>
+      </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -2509,7 +2662,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -2520,7 +2673,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -2530,8 +2683,17 @@
       <c r="C50">
         <v>720</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M50" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="N50" s="5">
+        <v>35</v>
+      </c>
+      <c r="O50" s="6">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2541,8 +2703,17 @@
       <c r="C51">
         <v>460</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M51" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="N51" s="5">
+        <v>345</v>
+      </c>
+      <c r="O51" s="6">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>73</v>
       </c>
@@ -2553,7 +2724,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -2564,7 +2735,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -2574,8 +2745,16 @@
       <c r="C54">
         <v>650</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <f>N51*2+N50</f>
+        <v>725</v>
+      </c>
+      <c r="O54">
+        <f>O50+O51*2</f>
+        <v>6810</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -2585,8 +2764,12 @@
       <c r="C55">
         <v>1200</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <f>O54/5</f>
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -2597,7 +2780,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -2608,7 +2791,7 @@
         <v>4820</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -2619,7 +2802,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -2630,7 +2813,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -2641,7 +2824,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -2652,7 +2835,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -2663,7 +2846,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -2674,7 +2857,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -2896,7 +3079,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I40 E2:E43 A2:A83">
-    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M50:M51">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">

</xml_diff>